<commit_message>
Added Bimanual Dexterity results, initial
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D535EF-6B49-4292-8DC6-CA07A8155F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3870E-DD0E-4791-A8BD-B5124F8ABE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
     <sheet name="tool_path_length" sheetId="2" r:id="rId2"/>
     <sheet name="tool_velocity" sheetId="3" r:id="rId3"/>
     <sheet name="tool_grasps" sheetId="4" r:id="rId4"/>
+    <sheet name="tool_bimanual" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="113">
   <si>
     <t>Author</t>
   </si>
@@ -316,6 +317,66 @@
   </si>
   <si>
     <t>Laparoscopic training workshop, values estimated from barplots, did not report SD so I used expert's difference from the ideal (5) number of grasps as SD</t>
+  </si>
+  <si>
+    <t>Movement-level process modeling of microsurgical bimanual and unimanual tasks</t>
+  </si>
+  <si>
+    <t>International Journal of Computer Assisted Radiology and Surgery</t>
+  </si>
+  <si>
+    <t>Bimanual efficiency defined as using both hand simultaneously for something productive</t>
+  </si>
+  <si>
+    <t>Hofstad et al.</t>
+  </si>
+  <si>
+    <t>Psychomotor skills assessment by motion analysis in minimally invasive surgery on an animal organ</t>
+  </si>
+  <si>
+    <t>Minimally Invasive Therapy and Allied Technologies</t>
+  </si>
+  <si>
+    <t>box trained</t>
+  </si>
+  <si>
+    <t>Bimanual dexterity defined as the correlation between the two hands tool movements. Values estimated from boxplots</t>
+  </si>
+  <si>
+    <t>Demirel et al.</t>
+  </si>
+  <si>
+    <t>Scoring metrics for assessing skills in arthroscopic rotator cuff repair: performance comparison study of novice and expert surgeons</t>
+  </si>
+  <si>
+    <t>Affordable, web-based surgical skill training and evaluation tool</t>
+  </si>
+  <si>
+    <t>Islam et al.</t>
+  </si>
+  <si>
+    <t>Journal of Biomedical Informatics</t>
+  </si>
+  <si>
+    <t>Standard deviations estimated from the standard deviations of other metrics, not given directly in the paper</t>
+  </si>
+  <si>
+    <t>Fundamentals of laparoscopy (FLS) training set</t>
+  </si>
+  <si>
+    <t>Mean values estimated from boxplot. Standard deviations were not given, I used the similar-ish values as in our study (i = 0), so novice's SD is about 1/5 of the mean, experts is 1/12</t>
+  </si>
+  <si>
+    <t>Zulbaran-Rojas et al.</t>
+  </si>
+  <si>
+    <t>Utilization of Flexible-Wearable Sensors to Describe the Kinematics of Surgical Proficiency</t>
+  </si>
+  <si>
+    <t>Vascular anastomosis</t>
+  </si>
+  <si>
+    <t>I took the ratio of number of dominant and non-dominant hand movements as measure of bimanual dexterity. Other options were velocity and path length. No. Movements felt closest to our definition.</t>
   </si>
 </sst>
 </file>
@@ -801,19 +862,19 @@
         <v>102.14</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O2:O15" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O15" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>99.449960080434423</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P2:P15" si="1">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P15" si="1">(J3-M3)/O3</f>
         <v>0.71895453695679024</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q2:Q15" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q15" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>0.70343753256203934</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R2:R15" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R15" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.33937031474894647</v>
       </c>
     </row>
@@ -1685,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B2A652-0C22-4014-BA4E-6ABE2842051B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="A1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,4 +1931,370 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAD4D7-D2C2-4F90-9A16-48DE70F95F03}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2">
+        <f>0.78316-0.25485</f>
+        <v>0.52830999999999995</v>
+      </c>
+      <c r="K2">
+        <v>9.4689999999999996E-2</v>
+      </c>
+      <c r="L2">
+        <v>25</v>
+      </c>
+      <c r="M2">
+        <v>0.78315999999999997</v>
+      </c>
+      <c r="N2">
+        <v>6.6960000000000006E-2</v>
+      </c>
+      <c r="O2">
+        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>8.2005602552508564E-2</v>
+      </c>
+      <c r="P2">
+        <f>(J2-M2)/O2</f>
+        <v>-3.1077144983700156</v>
+      </c>
+      <c r="Q2">
+        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>-3.0589022287621095</v>
+      </c>
+      <c r="R2">
+        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.42021291512017095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3">
+        <v>2017</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>28</v>
+      </c>
+      <c r="J3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.05</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0.24</v>
+      </c>
+      <c r="N3">
+        <v>0.13</v>
+      </c>
+      <c r="O3">
+        <f>SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>5.4902511001644679E-2</v>
+      </c>
+      <c r="P3">
+        <f>(J3-M3)/O3</f>
+        <v>-3.0963975399031822</v>
+      </c>
+      <c r="Q3">
+        <f>P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>-3.012711119905799</v>
+      </c>
+      <c r="R3">
+        <f>SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.83397177078499507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>2.93</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>14</v>
+      </c>
+      <c r="M4">
+        <v>4.5</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+      <c r="O4">
+        <f>SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>0.74620250724463644</v>
+      </c>
+      <c r="P4">
+        <f>(J4-M4)/O4</f>
+        <v>-2.1039864979779384</v>
+      </c>
+      <c r="Q4">
+        <f>P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>-2.0314352394269752</v>
+      </c>
+      <c r="R4">
+        <f>SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.51347124660338606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>2016</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <f>J5/5</f>
+        <v>6.2</v>
+      </c>
+      <c r="L5">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>88</v>
+      </c>
+      <c r="N5">
+        <f>M5/12</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="O5">
+        <f>SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>6.4238135182272424</v>
+      </c>
+      <c r="P5">
+        <f>(J5-M5)/O5</f>
+        <v>-8.8732339191144654</v>
+      </c>
+      <c r="Q5">
+        <f>P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>-8.6969445035029196</v>
+      </c>
+      <c r="R5">
+        <f>SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>1.067908470933508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>0.43</v>
+      </c>
+      <c r="K6">
+        <v>0.2</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>0.72</v>
+      </c>
+      <c r="N6">
+        <v>0.4</v>
+      </c>
+      <c r="O6">
+        <f>SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <v>0.33665016461206926</v>
+      </c>
+      <c r="P6">
+        <f>(J6-M6)/O6</f>
+        <v>-0.86142836238970666</v>
+      </c>
+      <c r="Q6">
+        <f>P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <v>-0.82502998088028245</v>
+      </c>
+      <c r="R6">
+        <f>SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <v>0.47632426341891154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added pupil analysis, removed drapery plots for now.
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3870E-DD0E-4791-A8BD-B5124F8ABE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE5C68-D89D-4C25-BEA6-6B38BC4A41D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="tool_velocity" sheetId="3" r:id="rId3"/>
     <sheet name="tool_grasps" sheetId="4" r:id="rId4"/>
     <sheet name="tool_bimanual" sheetId="5" r:id="rId5"/>
+    <sheet name="pupil_dilation" sheetId="6" r:id="rId6"/>
+    <sheet name="pupil_blinks" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="151">
   <si>
     <t>Author</t>
   </si>
@@ -377,6 +379,120 @@
   </si>
   <si>
     <t>I took the ratio of number of dominant and non-dominant hand movements as measure of bimanual dexterity. Other options were velocity and path length. No. Movements felt closest to our definition.</t>
+  </si>
+  <si>
+    <t>Castner et al.</t>
+  </si>
+  <si>
+    <t>Pupil diameter differentiates expertise in dental radiography visual search</t>
+  </si>
+  <si>
+    <t>PLOS ONE</t>
+  </si>
+  <si>
+    <t>Radiography</t>
+  </si>
+  <si>
+    <t>Dental radiography, visual search</t>
+  </si>
+  <si>
+    <t>Reported values are medians? Median change from baseline</t>
+  </si>
+  <si>
+    <t>Cabrera-Mino et al.</t>
+  </si>
+  <si>
+    <t>Task-Evoked Pupillary Responses in Nursing Simulation as an Indicator of Stress and Cognitive Load</t>
+  </si>
+  <si>
+    <t>Clinical Simulation in Nursing</t>
+  </si>
+  <si>
+    <t>Various nursing tasks</t>
+  </si>
+  <si>
+    <t>Elevate HOB</t>
+  </si>
+  <si>
+    <t>There were different tasks, picked the one that had the most significant result. Values estimated from barplot</t>
+  </si>
+  <si>
+    <t>Bednarik et al.</t>
+  </si>
+  <si>
+    <t>Pupil Size As an Indicator of Visual-motor Workload and Expertise in Microsurgical Training Tasks</t>
+  </si>
+  <si>
+    <t>Proceedings of the 2018 ACM Symposium on Eye Tracking Research &amp; Applications</t>
+  </si>
+  <si>
+    <t>Suturing</t>
+  </si>
+  <si>
+    <t>Took the segment 'needle push', estimated from plots</t>
+  </si>
+  <si>
+    <t>Gunawardena et al.</t>
+  </si>
+  <si>
+    <t>Assessing Surgeons’ Skill Level in Laparoscopic Cholecystectomy using Eye Metrics</t>
+  </si>
+  <si>
+    <t>Eye Tracking Research and Applications Symposium (ETRA)</t>
+  </si>
+  <si>
+    <t>Laparoscopic cholecystectomy</t>
+  </si>
+  <si>
+    <t>Study had only 4 participants of 3 skill levels who completed &gt;=7 tasks each. I picked the least experienced participant and expert E-2.</t>
+  </si>
+  <si>
+    <t>Zheng et al.</t>
+  </si>
+  <si>
+    <t>Action-related eye measures to assess surgical expertise</t>
+  </si>
+  <si>
+    <t>BJS Open</t>
+  </si>
+  <si>
+    <t>Box trainer</t>
+  </si>
+  <si>
+    <t>Transporting and loading task</t>
+  </si>
+  <si>
+    <t>Visual behaviour in robotic surgery—Demonstrating the validity of the simulated environment</t>
+  </si>
+  <si>
+    <t>Dilley et al.</t>
+  </si>
+  <si>
+    <t>International Journal of Medical Robotics and Computer Assisted Surgery</t>
+  </si>
+  <si>
+    <t>Robotic surgery</t>
+  </si>
+  <si>
+    <t>Fundamentals of Robotic Surgery, simulator task</t>
+  </si>
+  <si>
+    <t>SDs calculated from inter-quartile ranges (SD = (3/4)*IQR). The paper reports medians.</t>
+  </si>
+  <si>
+    <t>Gao et al.</t>
+  </si>
+  <si>
+    <t>American Surgeon</t>
+  </si>
+  <si>
+    <t>Quantitative evaluations of the effects of noise on mental workloads based on pupil dilation during laparoscopic surgery</t>
+  </si>
+  <si>
+    <t>Appendectromy simulator</t>
+  </si>
+  <si>
+    <t>They evaluated different noise conditions, I picked values from the no-noise condition. Paper does not give explicitly the number of participants in groups, only total number (24) which was "divided into experienced and moderately experienced". I assumed 12 per group</t>
   </si>
 </sst>
 </file>
@@ -694,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,19 +978,19 @@
         <v>102.14</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O15" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O16" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>99.449960080434423</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P15" si="1">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P16" si="1">(J3-M3)/O3</f>
         <v>0.71895453695679024</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q15" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q16" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>0.70343753256203934</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R15" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R16" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.33937031474894647</v>
       </c>
     </row>
@@ -1593,6 +1709,66 @@
       <c r="R15">
         <f t="shared" si="3"/>
         <v>0.53655897116915763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <v>6.2960000000000003</v>
+      </c>
+      <c r="K16">
+        <v>1.853</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>2.96</v>
+      </c>
+      <c r="N16">
+        <v>0.752</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>1.6336404133101019</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>2.0420650547206756</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>1.9382312383789464</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0.63716659150087573</v>
       </c>
     </row>
   </sheetData>
@@ -1937,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAD4D7-D2C2-4F90-9A16-48DE70F95F03}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2297,4 +2473,573 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298FF69-1A01-44B7-9B68-125032E688E1}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2">
+        <f>50*20</f>
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>0.314</v>
+      </c>
+      <c r="K2">
+        <v>0.315</v>
+      </c>
+      <c r="L2">
+        <f>26*15</f>
+        <v>390</v>
+      </c>
+      <c r="M2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="N2">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="O2">
+        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>0.32609677052433023</v>
+      </c>
+      <c r="P2">
+        <f>(J2-M2)/O2</f>
+        <v>0.78810961416996039</v>
+      </c>
+      <c r="Q2">
+        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>0.78768368571697722</v>
+      </c>
+      <c r="R2">
+        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>6.1542878227187438E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3">
+        <v>2019</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>0.75</v>
+      </c>
+      <c r="K3">
+        <v>0.75</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3">
+        <v>0.25</v>
+      </c>
+      <c r="N3">
+        <v>0.4</v>
+      </c>
+      <c r="O3">
+        <f>SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>0.58802145434433839</v>
+      </c>
+      <c r="P3">
+        <f>(J3-M3)/O3</f>
+        <v>0.8503091108427584</v>
+      </c>
+      <c r="Q3">
+        <f>P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>0.82554282606093055</v>
+      </c>
+      <c r="R3">
+        <f>SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.39560196502581091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <f>0.02/8</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L4">
+        <v>60</v>
+      </c>
+      <c r="M4">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="N4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O4">
+        <f>SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P4">
+        <f>(J4-M4)/O4</f>
+        <v>-3</v>
+      </c>
+      <c r="Q4">
+        <f>P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>-2.9791183294663575</v>
+      </c>
+      <c r="R4">
+        <f>SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.27852424952911653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>4.87</v>
+      </c>
+      <c r="K5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N5">
+        <v>0.31</v>
+      </c>
+      <c r="O5">
+        <f>SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>0.45260357930533429</v>
+      </c>
+      <c r="P5">
+        <f>(J5-M5)/O5</f>
+        <v>1.7012680305838788</v>
+      </c>
+      <c r="Q5">
+        <f>P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>1.5926764541636311</v>
+      </c>
+      <c r="R5">
+        <f>SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>0.62376486274553433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6">
+        <v>2020</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>3.25</v>
+      </c>
+      <c r="K6">
+        <f>0.96*(3/4)</f>
+        <v>0.72</v>
+      </c>
+      <c r="L6">
+        <v>14</v>
+      </c>
+      <c r="M6">
+        <v>3.26</v>
+      </c>
+      <c r="N6">
+        <f>0.7*(3/4)</f>
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="O6">
+        <f>SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <v>0.6428044025984887</v>
+      </c>
+      <c r="P6">
+        <f>(J6-M6)/O6</f>
+        <v>-1.5556831844299035E-2</v>
+      </c>
+      <c r="Q6">
+        <f>P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <v>-1.5164642806207463E-2</v>
+      </c>
+      <c r="R6">
+        <f>SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <v>0.35635362839287621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>0.108</v>
+      </c>
+      <c r="K7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O7">
+        <f>SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <v>5.5470712993434652E-2</v>
+      </c>
+      <c r="P7">
+        <f>(J7-M7)/O7</f>
+        <v>1.2619271724213279</v>
+      </c>
+      <c r="Q7">
+        <f>P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <v>1.218412442337834</v>
+      </c>
+      <c r="R7">
+        <f>SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <v>0.44703794088830068</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9C3E7-A606-4632-BFE8-84337DA69629}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>22.7</v>
+      </c>
+      <c r="K2">
+        <f>(3/4)*20.87</f>
+        <v>15.6525</v>
+      </c>
+      <c r="L2">
+        <v>14</v>
+      </c>
+      <c r="M2">
+        <v>25.28</v>
+      </c>
+      <c r="N2">
+        <f>(3/4)*20.08</f>
+        <v>15.059999999999999</v>
+      </c>
+      <c r="O2">
+        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>15.398549343201131</v>
+      </c>
+      <c r="P2">
+        <f>(J2-M2)/O2</f>
+        <v>-0.16754825032522563</v>
+      </c>
+      <c r="Q2">
+        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>-0.16332434485484179</v>
+      </c>
+      <c r="R2">
+        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.35696324528871254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tool movement results
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE5C68-D89D-4C25-BEA6-6B38BC4A41D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95A445-40EB-4F7E-AA5A-FC08B4AA4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="tool_grasps" sheetId="4" r:id="rId4"/>
     <sheet name="tool_bimanual" sheetId="5" r:id="rId5"/>
     <sheet name="pupil_dilation" sheetId="6" r:id="rId6"/>
-    <sheet name="pupil_blinks" sheetId="7" r:id="rId7"/>
+    <sheet name="tool_movements" sheetId="8" r:id="rId7"/>
+    <sheet name="pupil_blinks" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="177">
   <si>
     <t>Author</t>
   </si>
@@ -493,6 +494,84 @@
   </si>
   <si>
     <t>They evaluated different noise conditions, I picked values from the no-noise condition. Paper does not give explicitly the number of participants in groups, only total number (24) which was "divided into experienced and moderately experienced". I assumed 12 per group</t>
+  </si>
+  <si>
+    <t>Datta et al.</t>
+  </si>
+  <si>
+    <t>The use of electromagnetic motion tracking analysis to objectively measure open surgical skill in the laboratory-based model</t>
+  </si>
+  <si>
+    <t>Journal of the American College of Surgeons</t>
+  </si>
+  <si>
+    <t>Open surgery</t>
+  </si>
+  <si>
+    <t>Used ICSAD system to record data. Several skill groups, here we compare basic surgical trainees and consultants</t>
+  </si>
+  <si>
+    <t>Pagador et al.</t>
+  </si>
+  <si>
+    <t>Decomposition and analysis of laparoscopic suturing task using tool-motion analysis (TMA): Improving the objective assessment</t>
+  </si>
+  <si>
+    <t>Study reported left and right hand movements separately, I picked left hand</t>
+  </si>
+  <si>
+    <t>Bann et al.</t>
+  </si>
+  <si>
+    <t>Measurement of surgical dexterity using motion analysis of simple bench tasks</t>
+  </si>
+  <si>
+    <t>World Journal of Surgery</t>
+  </si>
+  <si>
+    <t>Knot tying and suturing</t>
+  </si>
+  <si>
+    <t>Used ICSAD system to record data. Reports medians and inter-quartile ranges.</t>
+  </si>
+  <si>
+    <t>Cholecystectomy</t>
+  </si>
+  <si>
+    <t>Multiple tasks, picked Calot's triangle. Surgeon groups A and C compared</t>
+  </si>
+  <si>
+    <t>Aggarwal et al.</t>
+  </si>
+  <si>
+    <t>An evaluation of the feasibility, validity, and reliability of laparoscopic skills assessment in the operating room</t>
+  </si>
+  <si>
+    <t>Annals of Surgery</t>
+  </si>
+  <si>
+    <t>Whole procedure, paper reports medians and inter-quartile ranges, the SDs are calculated from these (IQR*(3/4))</t>
+  </si>
+  <si>
+    <t>Yamaguchi et al.</t>
+  </si>
+  <si>
+    <t>Construct validity for eye-hand coordination skill on a virtual reality laparoscopic surgical simulator</t>
+  </si>
+  <si>
+    <t>LAP-mentor simulator</t>
+  </si>
+  <si>
+    <t>Effects and SDs estimated from barplots. Reported right hand movements</t>
+  </si>
+  <si>
+    <t>Goldbraikh</t>
+  </si>
+  <si>
+    <t>Video-based fully automatic assessment of open surgery suturing skills</t>
+  </si>
+  <si>
+    <t>Task:Balloon dominant hand</t>
   </si>
 </sst>
 </file>
@@ -810,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,19 +1057,19 @@
         <v>102.14</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O16" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O18" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>99.449960080434423</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P16" si="1">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P18" si="1">(J3-M3)/O3</f>
         <v>0.71895453695679024</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q16" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q18" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>0.70343753256203934</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R16" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R18" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.33937031474894647</v>
       </c>
     </row>
@@ -1769,6 +1848,185 @@
       <c r="R16">
         <f t="shared" si="3"/>
         <v>0.63716659150087573</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17">
+        <v>2001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>155</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>1236</v>
+      </c>
+      <c r="K17">
+        <v>202</v>
+      </c>
+      <c r="L17">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <v>782</v>
+      </c>
+      <c r="N17">
+        <v>201</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>201.47888011013657</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>2.2533379168666468</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="2"/>
+        <v>2.1790520514754386</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="3"/>
+        <v>0.511670837167987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18">
+        <v>2012</v>
+      </c>
+      <c r="D18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>108.07</v>
+      </c>
+      <c r="K18">
+        <v>6.93</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>30.07</v>
+      </c>
+      <c r="N18">
+        <v>13.37</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>10.648516328578362</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>7.3249641164247947</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="2"/>
+        <v>6.3695340142824302</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>1.9630190286092313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19">
+        <v>2007</v>
+      </c>
+      <c r="D19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>164</v>
+      </c>
+      <c r="H19" t="s">
+        <v>169</v>
+      </c>
+      <c r="I19">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>2175</v>
+      </c>
+      <c r="K19">
+        <f>(3127-1954)*(3/4)</f>
+        <v>879.75</v>
+      </c>
+      <c r="L19">
+        <v>33</v>
+      </c>
+      <c r="M19">
+        <v>1979</v>
+      </c>
+      <c r="N19">
+        <f>(2582-1137)*(3/4)</f>
+        <v>1083.75</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19" si="4">SQRT(((I19-1)*POWER(K19,2) + (L19-1)*POWER(N19,2))/((I19-1)+(L19-1)))</f>
+        <v>1028.9793304532409</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ref="P19" si="5">(J19-M19)/O19</f>
+        <v>0.19048001665268308</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" ref="Q19" si="6">P19*(1- (3/(4*(I19+L19)-9)))</f>
+        <v>0.18728761413895095</v>
+      </c>
+      <c r="R19">
+        <f t="shared" ref="R19" si="7">SQRT((I19+L19)/(I19*L19)+(POWER(P19,2)/(2*(I19+L19))))</f>
+        <v>0.31955842537614054</v>
       </c>
     </row>
   </sheetData>
@@ -1778,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0EBB68-8CAB-46D4-B803-BAB5987C358F}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1840,6 +2098,68 @@
       </c>
       <c r="R1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2">
+        <v>2007</v>
+      </c>
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>440</v>
+      </c>
+      <c r="K2">
+        <f>(565-391)*(3/4)</f>
+        <v>130.5</v>
+      </c>
+      <c r="L2">
+        <v>33</v>
+      </c>
+      <c r="M2">
+        <v>423</v>
+      </c>
+      <c r="N2">
+        <f>(667-274)*(3/4)</f>
+        <v>294.75</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>258.26236659645167</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>6.58245342673692E-2</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>6.4721329782441217E-2</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.31902616834043496</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +2243,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="A1:R2"/>
+      <selection activeCell="B2" sqref="B2:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2479,6 +2799,442 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298FF69-1A01-44B7-9B68-125032E688E1}">
   <dimension ref="A1:R7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="O2:R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2">
+        <f>50*20</f>
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>0.314</v>
+      </c>
+      <c r="K2">
+        <v>0.315</v>
+      </c>
+      <c r="L2">
+        <f>26*15</f>
+        <v>390</v>
+      </c>
+      <c r="M2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="N2">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O7" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>0.32609677052433023</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P7" si="1">(J2-M2)/O2</f>
+        <v>0.78810961416996039</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q7" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>0.78768368571697722</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2:R7" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>6.1542878227187438E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3">
+        <v>2019</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>0.75</v>
+      </c>
+      <c r="K3">
+        <v>0.75</v>
+      </c>
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3">
+        <v>0.25</v>
+      </c>
+      <c r="N3">
+        <v>0.4</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>0.58802145434433839</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>0.8503091108427584</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="2"/>
+        <v>0.82554282606093055</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="3"/>
+        <v>0.39560196502581091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <f>0.02/8</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L4">
+        <v>60</v>
+      </c>
+      <c r="M4">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="N4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>-2.9791183294663575</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>0.27852424952911653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>4.87</v>
+      </c>
+      <c r="K5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N5">
+        <v>0.31</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0.45260357930533429</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>1.7012680305838788</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>1.5926764541636311</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>0.62376486274553433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6">
+        <v>2020</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>3.25</v>
+      </c>
+      <c r="K6">
+        <f>0.96*(3/4)</f>
+        <v>0.72</v>
+      </c>
+      <c r="L6">
+        <v>14</v>
+      </c>
+      <c r="M6">
+        <v>3.26</v>
+      </c>
+      <c r="N6">
+        <f>0.7*(3/4)</f>
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0.6428044025984887</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>-1.5556831844299035E-2</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>-1.5164642806207463E-2</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>0.35635362839287621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>0.108</v>
+      </c>
+      <c r="K7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>5.5470712993434652E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>1.2619271724213279</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>1.218412442337834</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>0.44703794088830068</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2027-C5D7-4FCE-B720-F07DC782C0FB}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
@@ -2546,61 +3302,59 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2001</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="I2">
-        <f>50*20</f>
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="J2">
-        <v>0.314</v>
+        <v>2080</v>
       </c>
       <c r="K2">
-        <v>0.315</v>
+        <v>252</v>
       </c>
       <c r="L2">
-        <f>26*15</f>
-        <v>390</v>
+        <v>13</v>
       </c>
       <c r="M2">
-        <v>5.7000000000000002E-2</v>
+        <v>1337</v>
       </c>
       <c r="N2">
-        <v>0.35299999999999998</v>
+        <v>424</v>
       </c>
       <c r="O2">
-        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
-        <v>0.32609677052433023</v>
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>352.37430691512265</v>
       </c>
       <c r="P2">
-        <f>(J2-M2)/O2</f>
-        <v>0.78810961416996039</v>
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>2.1085532782018879</v>
       </c>
       <c r="Q2">
-        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
-        <v>0.78768368571697722</v>
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>2.039040532766661</v>
       </c>
       <c r="R2">
-        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
-        <v>6.1542878227187438E-2</v>
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.49917566927558565</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -2608,59 +3362,59 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="C3">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="I3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>0.75</v>
+        <v>176.5</v>
       </c>
       <c r="K3">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="L3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="M3">
-        <v>0.25</v>
+        <v>42.5</v>
       </c>
       <c r="N3">
-        <v>0.4</v>
+        <v>15.84</v>
       </c>
       <c r="O3">
-        <f>SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
-        <v>0.58802145434433839</v>
+        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>11.552177283958207</v>
       </c>
       <c r="P3">
-        <f>(J3-M3)/O3</f>
-        <v>0.8503091108427584</v>
+        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <v>11.59954497807764</v>
       </c>
       <c r="Q3">
-        <f>P3*(1- (3/(4*(I3+L3)-9)))</f>
-        <v>0.82554282606093055</v>
+        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>10.086560850502295</v>
       </c>
       <c r="R3">
-        <f>SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
-        <v>0.39560196502581091</v>
+        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>2.9848517938338057</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -2668,60 +3422,59 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J4">
-        <f>0.02/8</f>
-        <v>2.5000000000000001E-3</v>
+        <v>33.83</v>
       </c>
       <c r="K4">
-        <v>5.0000000000000001E-3</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="L4">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="M4">
-        <v>1.7500000000000002E-2</v>
+        <v>15.8</v>
       </c>
       <c r="N4">
-        <v>5.0000000000000001E-3</v>
+        <v>5.59</v>
       </c>
       <c r="O4">
         <f>SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
-        <v>5.0000000000000001E-3</v>
+        <v>13.287055731048923</v>
       </c>
       <c r="P4">
         <f>(J4-M4)/O4</f>
-        <v>-3</v>
+        <v>1.3569597633182089</v>
       </c>
       <c r="Q4">
         <f>P4*(1- (3/(4*(I4+L4)-9)))</f>
-        <v>-2.9791183294663575</v>
+        <v>1.3393369092491412</v>
       </c>
       <c r="R4">
         <f>SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
-        <v>0.27852424952911653</v>
+        <v>0.28637591552690278</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2729,59 +3482,61 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C5">
-        <v>2019</v>
+        <v>2003</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="I5">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J5">
-        <v>4.87</v>
+        <v>80</v>
       </c>
       <c r="K5">
-        <v>0.56000000000000005</v>
+        <f>(101-72)*(3/4)</f>
+        <v>21.75</v>
       </c>
       <c r="L5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M5">
-        <v>4.0999999999999996</v>
+        <v>57</v>
       </c>
       <c r="N5">
-        <v>0.31</v>
+        <f>(68-52)*(3/4)</f>
+        <v>12</v>
       </c>
       <c r="O5">
         <f>SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
-        <v>0.45260357930533429</v>
+        <v>17.896465632712431</v>
       </c>
       <c r="P5">
         <f>(J5-M5)/O5</f>
-        <v>1.7012680305838788</v>
+        <v>1.2851699588078982</v>
       </c>
       <c r="Q5">
         <f>P5*(1- (3/(4*(I5+L5)-9)))</f>
-        <v>1.5926764541636311</v>
+        <v>1.250435635596874</v>
       </c>
       <c r="R5">
         <f>SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
-        <v>0.62376486274553433</v>
+        <v>0.40181621231471359</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -2789,61 +3544,59 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2002</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>3.25</v>
+        <v>292.5</v>
       </c>
       <c r="K6">
-        <f>0.96*(3/4)</f>
-        <v>0.72</v>
+        <v>31.4</v>
       </c>
       <c r="L6">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M6">
-        <v>3.26</v>
+        <v>125.7</v>
       </c>
       <c r="N6">
-        <f>0.7*(3/4)</f>
-        <v>0.52499999999999991</v>
+        <v>17.2</v>
       </c>
       <c r="O6">
         <f>SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
-        <v>0.6428044025984887</v>
+        <v>27.111017552413497</v>
       </c>
       <c r="P6">
         <f>(J6-M6)/O6</f>
-        <v>-1.5556831844299035E-2</v>
+        <v>6.1524802482063619</v>
       </c>
       <c r="Q6">
         <f>P6*(1- (3/(4*(I6+L6)-9)))</f>
-        <v>-1.5164642806207463E-2</v>
+        <v>5.9403257568889014</v>
       </c>
       <c r="R6">
         <f>SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
-        <v>0.35635362839287621</v>
+        <v>0.98304741469556833</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -2851,59 +3604,177 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C7">
-        <v>2018</v>
+        <v>2007</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="H7" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J7">
-        <v>0.108</v>
+        <v>1708</v>
       </c>
       <c r="K7">
-        <v>7.4999999999999997E-2</v>
+        <f>(2303-1015)*(3/4)</f>
+        <v>966</v>
       </c>
       <c r="L7">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="M7">
-        <v>3.7999999999999999E-2</v>
+        <v>1771</v>
       </c>
       <c r="N7">
-        <v>2.3E-2</v>
+        <f>(2303-1015)*(3/4)</f>
+        <v>966</v>
       </c>
       <c r="O7">
         <f>SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
-        <v>5.5470712993434652E-2</v>
+        <v>966</v>
       </c>
       <c r="P7">
         <f>(J7-M7)/O7</f>
-        <v>1.2619271724213279</v>
+        <v>-6.5217391304347824E-2</v>
       </c>
       <c r="Q7">
         <f>P7*(1- (3/(4*(I7+L7)-9)))</f>
-        <v>1.218412442337834</v>
+        <v>-6.4124362399805679E-2</v>
       </c>
       <c r="R7">
         <f>SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
-        <v>0.44703794088830068</v>
+        <v>0.3190248418076812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8">
+        <v>2007</v>
+      </c>
+      <c r="D8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>37</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>16</v>
+      </c>
+      <c r="M8">
+        <v>31</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <f>SQRT(((I8-1)*POWER(K8,2) + (L8-1)*POWER(N8,2))/((I8-1)+(L8-1)))</f>
+        <v>2.5325467623418674</v>
+      </c>
+      <c r="P8">
+        <f>(J8-M8)/O8</f>
+        <v>2.3691566486423925</v>
+      </c>
+      <c r="Q8">
+        <f>P8*(1- (3/(4*(I8+L8)-9)))</f>
+        <v>2.3073525621560691</v>
+      </c>
+      <c r="R8">
+        <f>SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
+        <v>0.46871885374613781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9">
+        <f>2*12</f>
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <f>13*2</f>
+        <v>26</v>
+      </c>
+      <c r="M9">
+        <v>62</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <f>SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <v>14.306903927824496</v>
+      </c>
+      <c r="P9">
+        <f>(J9-M9)/O9</f>
+        <v>2.6560603322495555</v>
+      </c>
+      <c r="Q9">
+        <f>P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <v>2.614342107135688</v>
+      </c>
+      <c r="R9">
+        <f>SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <v>0.38816848147898525</v>
       </c>
     </row>
   </sheetData>
@@ -2911,7 +3782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9C3E7-A606-4632-BFE8-84337DA69629}">
   <dimension ref="A1:R2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added tool path length analysis
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95A445-40EB-4F7E-AA5A-FC08B4AA4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A0B172-3119-425D-AF5D-A5FBA6EB75F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="187">
   <si>
     <t>Author</t>
   </si>
@@ -572,6 +572,36 @@
   </si>
   <si>
     <t>Task:Balloon dominant hand</t>
+  </si>
+  <si>
+    <t>Task-Level vs . Segment-Level Quantitative Metrics for Surgical Skill Assessment</t>
+  </si>
+  <si>
+    <t>Effects and SDs estimated from barplots. Paper does not give Ne/Nn directly, total of 135 trials performed by 14 novices and 4 experts, so I estimated sample sizes by 135*(14/(14+4)) for novices and 135*(4/(14+4)) for experts</t>
+  </si>
+  <si>
+    <t>Wilson et al.</t>
+  </si>
+  <si>
+    <t>Psychomotor control in a virtual laparoscopic surgery training environment: Gaze control parameters differentiate novices from experts</t>
+  </si>
+  <si>
+    <t>LapMentor</t>
+  </si>
+  <si>
+    <t>reported left and right hand separately, I used left hand because usually differences are larger with non-dominant hand (all were right-handed)</t>
+  </si>
+  <si>
+    <t>Jimbo et al.</t>
+  </si>
+  <si>
+    <t>A new innovative laparoscopic fundoplication training simulator with a surgical skill validation system</t>
+  </si>
+  <si>
+    <t>Estimated effects and SDs from barplots. Reports left/right hand separately, I used left hand results</t>
+  </si>
+  <si>
+    <t>A study of psychomotor skills in minimally invasive surgery: What differentiates expert and nonexpert performance</t>
   </si>
 </sst>
 </file>
@@ -889,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2029,6 +2059,121 @@
         <v>0.31955842537614054</v>
       </c>
     </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20">
+        <v>2010</v>
+      </c>
+      <c r="D20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>74.5</v>
+      </c>
+      <c r="K20">
+        <v>13.44</v>
+      </c>
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>56.56</v>
+      </c>
+      <c r="N20">
+        <v>11.93</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ref="O20:O21" si="8">SQRT(((I20-1)*POWER(K20,2) + (L20-1)*POWER(N20,2))/((I20-1)+(L20-1)))</f>
+        <v>12.581210527343277</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ref="P20:P21" si="9">(J20-M20)/O20</f>
+        <v>1.4259359193624681</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ref="Q20:Q21" si="10">P20*(1- (3/(4*(I20+L20)-9)))</f>
+        <v>1.334918733020183</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ref="R20:R21" si="11">SQRT((I20+L20)/(I20*L20)+(POWER(P20,2)/(2*(I20+L20))))</f>
+        <v>0.60355967608829919</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21">
+        <v>2013</v>
+      </c>
+      <c r="D21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21">
+        <v>11</v>
+      </c>
+      <c r="J21">
+        <v>4.5</v>
+      </c>
+      <c r="K21">
+        <f>3*(3/4)</f>
+        <v>2.25</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21">
+        <v>1.9</v>
+      </c>
+      <c r="N21">
+        <v>0.4</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="8"/>
+        <v>1.7955674590502024</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="9"/>
+        <v>1.4480102025101951</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="10"/>
+        <v>1.3790573357239952</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="11"/>
+        <v>0.54037841581818158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2036,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0EBB68-8CAB-46D4-B803-BAB5987C358F}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,6 +2305,360 @@
       <c r="R2">
         <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
         <v>0.31902616834043496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
+        <v>2004</v>
+      </c>
+      <c r="D3">
+        <v>2004</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>10050</v>
+      </c>
+      <c r="K3">
+        <v>7554.5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>1299.23</v>
+      </c>
+      <c r="N3">
+        <v>437.7</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>6351.4868544117062</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <v>1.3777514148394665</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>1.3160610529809829</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.54179548524236587</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>1329.5</v>
+      </c>
+      <c r="K4">
+        <v>403.9</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>422.7</v>
+      </c>
+      <c r="N4">
+        <v>117.3</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>329.87375408838398</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <v>2.7489304279631734</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>2.6541397235506503</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.57897092311695464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5">
+        <v>2012</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>203.06</v>
+      </c>
+      <c r="K5">
+        <v>16.79</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>55.54</v>
+      </c>
+      <c r="N5">
+        <v>23.47</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O6" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>20.405207668632045</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P6" si="13">(J5-M5)/O5</f>
+        <v>7.229527010733416</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q6" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>6.2865452267247095</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R6" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>1.9407804615496191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>12000</v>
+      </c>
+      <c r="K6">
+        <v>2500</v>
+      </c>
+      <c r="L6">
+        <v>26</v>
+      </c>
+      <c r="M6">
+        <v>8000</v>
+      </c>
+      <c r="N6">
+        <v>1250</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="12"/>
+        <v>1951.5618744994995</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="13"/>
+        <v>2.0496403687051155</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="14"/>
+        <v>2.0174470644846165</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="15"/>
+        <v>0.34948313484124172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7">
+        <v>2017</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>185</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>15000</v>
+      </c>
+      <c r="K7">
+        <f>9000*(3/4)</f>
+        <v>6750</v>
+      </c>
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>10000</v>
+      </c>
+      <c r="N7">
+        <f>4000*(3/4)</f>
+        <v>3000</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7" si="16">SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <v>5632.7649108178248</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7" si="17">(J7-M7)/O7</f>
+        <v>0.88766353277009868</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7" si="18">P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <v>0.86954795046866806</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7" si="19">SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <v>0.34414417348878751</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <v>2013</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <f>5*(3/4)</f>
+        <v>3.75</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>3.5</v>
+      </c>
+      <c r="N8">
+        <v>0.5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8" si="20">SQRT(((I8-1)*POWER(K8,2) + (L8-1)*POWER(N8,2))/((I8-1)+(L8-1)))</f>
+        <v>2.980404754391591</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8" si="21">(J8-M8)/O8</f>
+        <v>0.83881224398004317</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8" si="22">P8*(1- (3/(4*(I8+L8)-9)))</f>
+        <v>0.79886880379051728</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8" si="23">SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
+        <v>0.50329995463924693</v>
       </c>
     </row>
   </sheetData>
@@ -2434,7 +2933,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:R2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3233,10 +3732,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2027-C5D7-4FCE-B720-F07DC782C0FB}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3461,19 +3960,19 @@
         <v>5.59</v>
       </c>
       <c r="O4">
-        <f>SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <f t="shared" ref="O4:O10" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
         <v>13.287055731048923</v>
       </c>
       <c r="P4">
-        <f>(J4-M4)/O4</f>
+        <f t="shared" ref="P4:P10" si="9">(J4-M4)/O4</f>
         <v>1.3569597633182089</v>
       </c>
       <c r="Q4">
-        <f>P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <f t="shared" ref="Q4:Q10" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
         <v>1.3393369092491412</v>
       </c>
       <c r="R4">
-        <f>SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <f t="shared" ref="R4:R10" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
         <v>0.28637591552690278</v>
       </c>
     </row>
@@ -3523,19 +4022,19 @@
         <v>12</v>
       </c>
       <c r="O5">
-        <f>SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <f t="shared" si="8"/>
         <v>17.896465632712431</v>
       </c>
       <c r="P5">
-        <f>(J5-M5)/O5</f>
+        <f t="shared" si="9"/>
         <v>1.2851699588078982</v>
       </c>
       <c r="Q5">
-        <f>P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <f t="shared" si="10"/>
         <v>1.250435635596874</v>
       </c>
       <c r="R5">
-        <f>SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <f t="shared" si="11"/>
         <v>0.40181621231471359</v>
       </c>
     </row>
@@ -3583,19 +4082,19 @@
         <v>17.2</v>
       </c>
       <c r="O6">
-        <f>SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <f t="shared" si="8"/>
         <v>27.111017552413497</v>
       </c>
       <c r="P6">
-        <f>(J6-M6)/O6</f>
+        <f t="shared" si="9"/>
         <v>6.1524802482063619</v>
       </c>
       <c r="Q6">
-        <f>P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <f t="shared" si="10"/>
         <v>5.9403257568889014</v>
       </c>
       <c r="R6">
-        <f>SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <f t="shared" si="11"/>
         <v>0.98304741469556833</v>
       </c>
     </row>
@@ -3645,19 +4144,19 @@
         <v>966</v>
       </c>
       <c r="O7">
-        <f>SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <f t="shared" si="8"/>
         <v>966</v>
       </c>
       <c r="P7">
-        <f>(J7-M7)/O7</f>
+        <f t="shared" si="9"/>
         <v>-6.5217391304347824E-2</v>
       </c>
       <c r="Q7">
-        <f>P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <f t="shared" si="10"/>
         <v>-6.4124362399805679E-2</v>
       </c>
       <c r="R7">
-        <f>SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <f t="shared" si="11"/>
         <v>0.3190248418076812</v>
       </c>
     </row>
@@ -3705,19 +4204,19 @@
         <v>2</v>
       </c>
       <c r="O8">
-        <f>SQRT(((I8-1)*POWER(K8,2) + (L8-1)*POWER(N8,2))/((I8-1)+(L8-1)))</f>
+        <f t="shared" si="8"/>
         <v>2.5325467623418674</v>
       </c>
       <c r="P8">
-        <f>(J8-M8)/O8</f>
+        <f t="shared" si="9"/>
         <v>2.3691566486423925</v>
       </c>
       <c r="Q8">
-        <f>P8*(1- (3/(4*(I8+L8)-9)))</f>
+        <f t="shared" si="10"/>
         <v>2.3073525621560691</v>
       </c>
       <c r="R8">
-        <f>SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
+        <f t="shared" si="11"/>
         <v>0.46871885374613781</v>
       </c>
     </row>
@@ -3761,20 +4260,199 @@
         <v>5</v>
       </c>
       <c r="O9">
-        <f>SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <f t="shared" si="8"/>
         <v>14.306903927824496</v>
       </c>
       <c r="P9">
-        <f>(J9-M9)/O9</f>
+        <f t="shared" si="9"/>
         <v>2.6560603322495555</v>
       </c>
       <c r="Q9">
-        <f>P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <f t="shared" si="10"/>
         <v>2.614342107135688</v>
       </c>
       <c r="R9">
-        <f>SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <f t="shared" si="11"/>
         <v>0.38816848147898525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>2016</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10">
+        <f>(14/18)*135</f>
+        <v>105</v>
+      </c>
+      <c r="J10">
+        <v>725</v>
+      </c>
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>30</v>
+      </c>
+      <c r="M10">
+        <v>425</v>
+      </c>
+      <c r="N10">
+        <v>25</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="8"/>
+        <v>45.729262114469272</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="9"/>
+        <v>6.5603507716577933</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="10"/>
+        <v>6.5232866430043597</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="11"/>
+        <v>0.44973091056854569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>26.83</v>
+      </c>
+      <c r="K11">
+        <v>7.91</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>22.59</v>
+      </c>
+      <c r="N11">
+        <v>5.61</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:O12" si="12">SQRT(((I11-1)*POWER(K11,2) + (L11-1)*POWER(N11,2))/((I11-1)+(L11-1)))</f>
+        <v>6.6654907296212382</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P12" si="13">(J11-M11)/O11</f>
+        <v>0.63611220418589243</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11:Q12" si="14">P11*(1- (3/(4*(I11+L11)-9)))</f>
+        <v>0.59550929753572912</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ref="R11:R12" si="15">SQRT((I11+L11)/(I11*L11)+(POWER(P11,2)/(2*(I11+L11))))</f>
+        <v>0.55327935991365229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <v>2013</v>
+      </c>
+      <c r="D12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>185</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>700</v>
+      </c>
+      <c r="K12">
+        <f>500*(3/4)</f>
+        <v>375</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>400</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="12"/>
+        <v>298.04047543915908</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="13"/>
+        <v>1.0065746927760519</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="14"/>
+        <v>0.95864256454862085</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="15"/>
+        <v>0.51177189546932644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added jerk results and extended others
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A0B172-3119-425D-AF5D-A5FBA6EB75F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA017A4-EFC4-42E1-A6F0-451DF93E9F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
     <sheet name="tool_path_length" sheetId="2" r:id="rId2"/>
-    <sheet name="tool_velocity" sheetId="3" r:id="rId3"/>
-    <sheet name="tool_grasps" sheetId="4" r:id="rId4"/>
-    <sheet name="tool_bimanual" sheetId="5" r:id="rId5"/>
-    <sheet name="pupil_dilation" sheetId="6" r:id="rId6"/>
-    <sheet name="tool_movements" sheetId="8" r:id="rId7"/>
-    <sheet name="pupil_blinks" sheetId="7" r:id="rId8"/>
+    <sheet name="tool_jerk" sheetId="10" r:id="rId3"/>
+    <sheet name="tool_velocity" sheetId="3" r:id="rId4"/>
+    <sheet name="tool_grasps" sheetId="4" r:id="rId5"/>
+    <sheet name="tool_bimanual" sheetId="5" r:id="rId6"/>
+    <sheet name="pupil_dilation" sheetId="6" r:id="rId7"/>
+    <sheet name="tool_movements" sheetId="8" r:id="rId8"/>
+    <sheet name="tool_idle" sheetId="11" r:id="rId9"/>
+    <sheet name="pupil_blinks" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="221">
   <si>
     <t>Author</t>
   </si>
@@ -602,6 +604,108 @@
   </si>
   <si>
     <t>A study of psychomotor skills in minimally invasive surgery: What differentiates expert and nonexpert performance</t>
+  </si>
+  <si>
+    <t>Ghasemloonia et al.</t>
+  </si>
+  <si>
+    <t>Modified O’Connor Dexterity board and Tweezer Dexterity pegboard</t>
+  </si>
+  <si>
+    <t>Results from task C included. Task had 4 groups of participants, results are from surgeons and residents. 9 trials per participant, 4 participants per group, so n=36 for both groups</t>
+  </si>
+  <si>
+    <t>Hwang et al.</t>
+  </si>
+  <si>
+    <t>Correlating motor performance with surgical error in laparoscopic cholecystectomy</t>
+  </si>
+  <si>
+    <t>Ebina et al.</t>
+  </si>
+  <si>
+    <t>Motion analysis for better understanding of psychomotor skills in laparoscopy: objective assessment-based simulation training using animal organs</t>
+  </si>
+  <si>
+    <t>Applying Hem-o-lock, suturing, suturing and knot tying</t>
+  </si>
+  <si>
+    <t>Results from task 3, knot tying and suturing. Results given in paper as medians and inter-quartile ranges</t>
+  </si>
+  <si>
+    <t>Azari et al.</t>
+  </si>
+  <si>
+    <t>Can surgical performance for varying experience be measured from hand motions?</t>
+  </si>
+  <si>
+    <t>Proceedings of the Human Factors and Ergonomics Society</t>
+  </si>
+  <si>
+    <t>Reported grand average results by skill group and by skill group and task. Results included here are the grand average by skill. Had 4 skill groups, picked medical students and attending surgeons. Paper did not report SDs for motion metrics, so I used the ratio of subjective evaluations mean and sd to estimate the sd. I.e. for novice's the subjective motion fluidity score was mean=4.1, sd=1.9, so the SD for jerk was calculated as 178.34*(1.9/4.1) (mean jerk * (sd of fluidity score / mean of fluidity score)</t>
+  </si>
+  <si>
+    <t>Davids et al.</t>
+  </si>
+  <si>
+    <t>Automated vision-based microsurgical skill analysis in neurosurgery using deep learning: Development and preclinical validation.</t>
+  </si>
+  <si>
+    <t>Arachnoid dissection</t>
+  </si>
+  <si>
+    <t>Values given as medians</t>
+  </si>
+  <si>
+    <t>Oropesa et al.</t>
+  </si>
+  <si>
+    <t>Relevance of Motion-Related Assessment Metrics in Laparoscopic Surgery</t>
+  </si>
+  <si>
+    <t>Surgical Innovation</t>
+  </si>
+  <si>
+    <t>Novel training tasks</t>
+  </si>
+  <si>
+    <t>Means and SDs estimated from boxplots. Reports dominant and non-dominant hand separately, I picked non-dominant hand. Results for Coordinated pulling task.</t>
+  </si>
+  <si>
+    <t>Pellen et al.</t>
+  </si>
+  <si>
+    <t>Laparoscopic surgical skills assessment: Can simulators replace experts?</t>
+  </si>
+  <si>
+    <t>Sharp dissection</t>
+  </si>
+  <si>
+    <t>Values estimated from boxplots</t>
+  </si>
+  <si>
+    <t>Maithel et al</t>
+  </si>
+  <si>
+    <t>Simulated laparoscopy using a head-mounted display vs traditional video monitor: An assessment of performance and muscle fatigue</t>
+  </si>
+  <si>
+    <t>Block moving training task</t>
+  </si>
+  <si>
+    <t>Liang et al.</t>
+  </si>
+  <si>
+    <t>Motion control skill assessment based on kinematic analysis of robotic end-effector movements</t>
+  </si>
+  <si>
+    <t>The International Journal of Medical Robotics and Computer Assisted Surgery</t>
+  </si>
+  <si>
+    <t>Ring-threading</t>
+  </si>
+  <si>
+    <t>Estimated from boxplots. Reported left/right hand separately, here the results are for left hand</t>
   </si>
 </sst>
 </file>
@@ -2179,12 +2283,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0EBB68-8CAB-46D4-B803-BAB5987C358F}">
-  <dimension ref="A1:R8"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9C3E7-A606-4632-BFE8-84337DA69629}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,6 +2354,139 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>22.7</v>
+      </c>
+      <c r="K2">
+        <f>(3/4)*20.87</f>
+        <v>15.6525</v>
+      </c>
+      <c r="L2">
+        <v>14</v>
+      </c>
+      <c r="M2">
+        <v>25.28</v>
+      </c>
+      <c r="N2">
+        <f>(3/4)*20.08</f>
+        <v>15.059999999999999</v>
+      </c>
+      <c r="O2">
+        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>15.398549343201131</v>
+      </c>
+      <c r="P2">
+        <f>(J2-M2)/O2</f>
+        <v>-0.16754825032522563</v>
+      </c>
+      <c r="Q2">
+        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>-0.16332434485484179</v>
+      </c>
+      <c r="R2">
+        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.35696324528871254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0EBB68-8CAB-46D4-B803-BAB5987C358F}">
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>166</v>
       </c>
       <c r="C2">
@@ -2659,6 +2896,130 @@
       <c r="R8">
         <f t="shared" ref="R8" si="23">SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
         <v>0.50329995463924693</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9">
+        <v>2013</v>
+      </c>
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>1000</v>
+      </c>
+      <c r="K9">
+        <f>900*(3/4)</f>
+        <v>675</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>800</v>
+      </c>
+      <c r="N9">
+        <f>800*(3/4)</f>
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O10" si="24">SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <v>663.08936049374222</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P10" si="25">(J9-M9)/O9</f>
+        <v>0.30161847243496448</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9:Q10" si="26">P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <v>0.2888740299377125</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ref="R9:R10" si="27">SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <v>0.5610475403857057</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10">
+        <v>2009</v>
+      </c>
+      <c r="D10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" t="s">
+        <v>212</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>1750</v>
+      </c>
+      <c r="K10">
+        <f>1000*(3/4)</f>
+        <v>750</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>500</v>
+      </c>
+      <c r="N10">
+        <f>400*(3/4)</f>
+        <v>300</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="24"/>
+        <v>571.18298293979308</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="25"/>
+        <v>2.1884405476620428</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="26"/>
+        <v>2.0959712287467451</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="27"/>
+        <v>0.565448318386644</v>
       </c>
     </row>
   </sheetData>
@@ -2667,6 +3028,554 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38582DD-83D6-42FC-BEAD-D85E565DA625}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2">
+        <v>2017</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2">
+        <v>36</v>
+      </c>
+      <c r="J2">
+        <v>1140</v>
+      </c>
+      <c r="K2">
+        <v>68</v>
+      </c>
+      <c r="L2">
+        <v>36</v>
+      </c>
+      <c r="M2">
+        <v>1043</v>
+      </c>
+      <c r="N2">
+        <v>41</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>56.14712815451918</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>1.7276039432159747</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>1.7090275567297815</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.27619205506685246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3">
+        <v>2006</v>
+      </c>
+      <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>19600</v>
+      </c>
+      <c r="K3">
+        <v>7410</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>2430</v>
+      </c>
+      <c r="N3">
+        <v>367</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>5246.0837297931112</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <v>3.2729176437824661</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>2.6183341150259731</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>1.2487323539955286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>32.4</v>
+      </c>
+      <c r="K4">
+        <f>(35.9-29.2)*(3/4)</f>
+        <v>5.0249999999999995</v>
+      </c>
+      <c r="L4">
+        <v>18</v>
+      </c>
+      <c r="M4">
+        <v>40.1</v>
+      </c>
+      <c r="N4">
+        <f>(48.5-35.4)*(3/4)</f>
+        <v>9.8250000000000011</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>8.0212004873375733</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <v>-0.95995605796855177</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>-0.93654249557907487</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.36903195024478913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>178.34</v>
+      </c>
+      <c r="K5">
+        <f>178.34*(1.9/4.1)</f>
+        <v>82.645365853658546</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>191.62</v>
+      </c>
+      <c r="N5">
+        <f>191.62*(1.5/7.1)</f>
+        <v>40.4830985915493</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>66.063252001145727</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5" si="13">(J5-M5)/O5</f>
+        <v>-0.2010194714569862</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>-0.19722665124081665</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>0.30973472993773743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>3264.98</v>
+      </c>
+      <c r="K6">
+        <v>21871</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>193.2</v>
+      </c>
+      <c r="N6">
+        <v>10161</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O8" si="16">SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <v>21871</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P8" si="17">(J6-M6)/O6</f>
+        <v>0.14044991084083946</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q8" si="18">P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <v>0.13065107985194369</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R8" si="19">SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <v>1.0411974032171929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7">
+        <v>2013</v>
+      </c>
+      <c r="D7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>350</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>375</v>
+      </c>
+      <c r="N7">
+        <v>40</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="16"/>
+        <v>24.494897427831781</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="17"/>
+        <v>-1.0206207261596576</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="18"/>
+        <v>-0.97749590674446085</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="19"/>
+        <v>0.58184333515703923</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8">
+        <v>2005</v>
+      </c>
+      <c r="D8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>215</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>3.06</v>
+      </c>
+      <c r="K8">
+        <v>0.22</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+      <c r="M8">
+        <v>2.76</v>
+      </c>
+      <c r="N8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="16"/>
+        <v>0.18136236570001973</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="17"/>
+        <v>1.654146927572679</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="18"/>
+        <v>1.6059678908472612</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="19"/>
+        <v>0.43869179913171907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="D9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" t="s">
+        <v>220</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="K9">
+        <f>0.4*(3/4)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>0.25</v>
+      </c>
+      <c r="N9">
+        <f>0.4*(3/4)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="20">SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9" si="21">(J9-M9)/O9</f>
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9" si="22">P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <v>0.15962441314553985</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ref="R9" si="23">SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <v>0.44798933519052042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AC6236-8F35-404B-A05E-33379B58B182}">
   <dimension ref="A1:R1"/>
   <sheetViews>
@@ -2737,7 +3646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B2A652-0C22-4014-BA4E-6ABE2842051B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -2928,7 +3837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAD4D7-D2C2-4F90-9A16-48DE70F95F03}">
   <dimension ref="A1:R6"/>
   <sheetViews>
@@ -3294,7 +4203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298FF69-1A01-44B7-9B68-125032E688E1}">
   <dimension ref="A1:R7"/>
   <sheetViews>
@@ -3730,12 +4639,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2027-C5D7-4FCE-B720-F07DC782C0FB}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4460,135 +5369,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9C3E7-A606-4632-BFE8-84337DA69629}">
-  <dimension ref="A1:R2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1CE573-6817-4853-A70A-1BB8041487EC}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2">
-        <v>2020</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2">
-        <v>18</v>
-      </c>
-      <c r="J2">
-        <v>22.7</v>
-      </c>
-      <c r="K2">
-        <f>(3/4)*20.87</f>
-        <v>15.6525</v>
-      </c>
-      <c r="L2">
-        <v>14</v>
-      </c>
-      <c r="M2">
-        <v>25.28</v>
-      </c>
-      <c r="N2">
-        <f>(3/4)*20.08</f>
-        <v>15.059999999999999</v>
-      </c>
-      <c r="O2">
-        <f>SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
-        <v>15.398549343201131</v>
-      </c>
-      <c r="P2">
-        <f>(J2-M2)/O2</f>
-        <v>-0.16754825032522563</v>
-      </c>
-      <c r="Q2">
-        <f>P2*(1- (3/(4*(I2+L2)-9)))</f>
-        <v>-0.16332434485484179</v>
-      </c>
-      <c r="R2">
-        <f>SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
-        <v>0.35696324528871254</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates, removed form from intro
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF91ACC-7D11-464D-A4E8-84A66271F7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC53D7E-4A54-4279-A791-7F2A250507E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="266">
   <si>
     <t>Author</t>
   </si>
@@ -793,6 +793,54 @@
   </si>
   <si>
     <t>Estimated effects and SDs from boxplots.</t>
+  </si>
+  <si>
+    <t>Validation of a novel virtual reality simulation system with the focus on training for surgical dissection during laparoscopic sigmoid colectomy</t>
+  </si>
+  <si>
+    <t>Mori et al.</t>
+  </si>
+  <si>
+    <t>BMC Surgery</t>
+  </si>
+  <si>
+    <t>Sigmoid Colectomy</t>
+  </si>
+  <si>
+    <t>Bimanual dexterity measured in GOALS score (see paper for more information). Results given as medians and inter-quartile ranges. SD calculated from IQR as SD = IQR*(3/4)</t>
+  </si>
+  <si>
+    <t>Pastewski et al.</t>
+  </si>
+  <si>
+    <t>Analysis of Instrument Motion and the Impact of Residency Level and Concurrent Distraction on Laparoscopic Skills</t>
+  </si>
+  <si>
+    <t>Peg transfer</t>
+  </si>
+  <si>
+    <t>Junior and Senior residents. Did task with and without secondary task (to add distractions). Velocity was reported for three degrees of freedom of motion (yaw, pitch, roll). Results here are for Roll and NO secondary task.</t>
+  </si>
+  <si>
+    <t>Results for needle holder (left hand), from task 3, knot tying and suturing. Results given in paper as medians and inter-quartile ranges</t>
+  </si>
+  <si>
+    <t>Bimanual carryinig</t>
+  </si>
+  <si>
+    <t>Estimated effects and SDs from barplots. Compared experts and novices post-training. Results are for bimanual carrying task, which was repeated 3 times by each participant (5 novices 5 experts)</t>
+  </si>
+  <si>
+    <t>Frasier et al.</t>
+  </si>
+  <si>
+    <t>A marker-less technique for measuring kinematics in the operating room</t>
+  </si>
+  <si>
+    <t>Surgery (United States)</t>
+  </si>
+  <si>
+    <t>Gives values for grand average and by different tasks. I used grand average results.</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -2689,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0EBB68-8CAB-46D4-B803-BAB5987C358F}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="A8" sqref="A8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3579,20 +3627,82 @@
         <v>225</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15" si="32">SQRT(((I15-1)*POWER(K15,2) + (L15-1)*POWER(N15,2))/((I15-1)+(L15-1)))</f>
+        <f t="shared" ref="O15:O16" si="32">SQRT(((I15-1)*POWER(K15,2) + (L15-1)*POWER(N15,2))/((I15-1)+(L15-1)))</f>
         <v>576.32998360314377</v>
       </c>
       <c r="P15">
-        <f t="shared" ref="P15" si="33">(J15-M15)/O15</f>
+        <f t="shared" ref="P15:P16" si="33">(J15-M15)/O15</f>
         <v>1.0410702498052837</v>
       </c>
       <c r="Q15">
-        <f t="shared" ref="Q15" si="34">P15*(1- (3/(4*(I15+L15)-9)))</f>
+        <f t="shared" ref="Q15:Q16" si="34">P15*(1- (3/(4*(I15+L15)-9)))</f>
         <v>1.0214274149032974</v>
       </c>
       <c r="R15">
-        <f t="shared" ref="R15" si="35">SQRT((I15+L15)/(I15*L15)+(POWER(P15,2)/(2*(I15+L15))))</f>
+        <f t="shared" ref="R15:R16" si="35">SQRT((I15+L15)/(I15*L15)+(POWER(P15,2)/(2*(I15+L15))))</f>
         <v>0.33017047922702103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="s">
+        <v>194</v>
+      </c>
+      <c r="H16" t="s">
+        <v>259</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K16">
+        <f>(14.9-6.9)*(3/4)</f>
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>18</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <f>(5.6-4.4)*(3/4)</f>
+        <v>0.89999999999999947</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="32"/>
+        <v>4.0868396181543671</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="33"/>
+        <v>0.92981383050115773</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="34"/>
+        <v>0.90713544439137339</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="35"/>
+        <v>0.36786073670199965</v>
       </c>
     </row>
   </sheetData>
@@ -4046,7 +4156,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4594,10 +4704,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AC6236-8F35-404B-A05E-33379B58B182}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4656,6 +4766,482 @@
       </c>
       <c r="R1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>190.38</v>
+      </c>
+      <c r="K2">
+        <v>133.91999999999999</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>116.38</v>
+      </c>
+      <c r="N2">
+        <v>94.4</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>133.91999999999999</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>0.55256869772998807</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>0.51401739323719819</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>1.0464592099878391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>15.11</v>
+      </c>
+      <c r="K3">
+        <v>1.46</v>
+      </c>
+      <c r="L3">
+        <v>23</v>
+      </c>
+      <c r="M3">
+        <v>16.14</v>
+      </c>
+      <c r="N3">
+        <v>1.37</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O4" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>1.4041021533858771</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P4" si="5">(J3-M3)/O3</f>
+        <v>-0.73356486030324841</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q4" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>-0.71773252518878983</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R4" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.34954068305795166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4">
+        <v>2006</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>566</v>
+      </c>
+      <c r="K4">
+        <v>83</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>85</v>
+      </c>
+      <c r="N4">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>62.900715417235119</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="5"/>
+        <v>7.6469718477669897</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="6"/>
+        <v>6.1175774782135921</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="7"/>
+        <v>2.3536528071726597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5">
+        <v>2021</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>1.7</v>
+      </c>
+      <c r="K5">
+        <f>(1.7-1.6)*(3/4)</f>
+        <v>7.49999999999999E-2</v>
+      </c>
+      <c r="L5">
+        <v>18</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <f>(2.4-1.8)*(3/4)</f>
+        <v>0.4499999999999999</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O6" si="8">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>0.33702924157618619</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P6" si="9">(J5-M5)/O5</f>
+        <v>-0.89013047828428382</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q6" si="10">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>-0.8684199788139354</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R6" si="11">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>0.36637038170610059</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6">
+        <v>2017</v>
+      </c>
+      <c r="D6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <f>6*(3/4)</f>
+        <v>4.5</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="M6">
+        <v>27</v>
+      </c>
+      <c r="N6">
+        <f>8*(3/4)</f>
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="8"/>
+        <v>5.1195175026030979</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="9"/>
+        <v>-0.78132363019877127</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="10"/>
+        <v>-0.76537824999063309</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="11"/>
+        <v>0.34082228272049281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>2009</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I7">
+        <f>5*3</f>
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <f>5*3</f>
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>34</v>
+      </c>
+      <c r="N7">
+        <v>0.5</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O8" si="12">SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <v>1.4577379737113252</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:P8" si="13">(J7-M7)/O7</f>
+        <v>0.68599434057003528</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q8" si="14">P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <v>0.66745395298706134</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R8" si="15">SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <v>0.37573457465108967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <v>2013</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <f>5*(3/4)</f>
+        <v>3.75</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>25</v>
+      </c>
+      <c r="N8">
+        <f>8*(3/4)</f>
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="12"/>
+        <v>4.7211293670053145</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="13"/>
+        <v>1.0590686277193835</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="14"/>
+        <v>1.0086367883041747</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="15"/>
+        <v>0.51470624777104745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>2016</v>
+      </c>
+      <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" t="s">
+        <v>265</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>219.22</v>
+      </c>
+      <c r="K9">
+        <v>60.81</v>
+      </c>
+      <c r="L9">
+        <v>39</v>
+      </c>
+      <c r="M9">
+        <v>386.7</v>
+      </c>
+      <c r="N9">
+        <v>172.87</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="16">SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <v>144.41024680665365</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9" si="17">(J9-M9)/O9</f>
+        <v>-1.1597514975805956</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9" si="18">P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <v>-1.1446897898198087</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ref="R9" si="19">SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <v>0.29063482710767857</v>
       </c>
     </row>
   </sheetData>
@@ -4856,10 +5442,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CAD4D7-D2C2-4F90-9A16-48DE70F95F03}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5212,6 +5798,73 @@
       <c r="R6">
         <f>SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
         <v>0.47632426341891154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H7" t="s">
+        <v>254</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>(2-1.25)*(3/4)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="L7">
+        <v>44</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <f>(4-3)*(3/4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O7">
+        <f>SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <v>0.73271088048083466</v>
+      </c>
+      <c r="P7">
+        <f>(J7-M7)/O7</f>
+        <v>-2.7295896011364245</v>
+      </c>
+      <c r="Q7">
+        <f>P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <v>-2.6867164660400409</v>
+      </c>
+      <c r="R7">
+        <f>SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <v>0.51371250062681983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -5661,7 +6314,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:R10"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added tool force results
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB32196F-829D-42B4-AE67-F92DBF1EFF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BFCC2B-F25F-48AB-A2C4-38C4FC848849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="pupil_dilation" sheetId="6" r:id="rId8"/>
     <sheet name="tool_movements" sheetId="8" r:id="rId9"/>
     <sheet name="pupil_blinks" sheetId="7" r:id="rId10"/>
+    <sheet name="scale_UWOMSAb" sheetId="12" r:id="rId11"/>
+    <sheet name="tool_force" sheetId="14" r:id="rId12"/>
+    <sheet name="scale_OSATS" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="302">
   <si>
     <t>Author</t>
   </si>
@@ -868,6 +871,87 @@
   </si>
   <si>
     <t>Values estimated from boxplot, used results for US hook</t>
+  </si>
+  <si>
+    <t>Values not reported directly in paper, calculated from data</t>
+  </si>
+  <si>
+    <t>Results for needle extraction phase (c), estimated from boxplot. Maximum needle gripping force</t>
+  </si>
+  <si>
+    <t>Prasad et al.</t>
+  </si>
+  <si>
+    <t>Objective Assessment of Laparoscopic Force and Psychomotor Skills in a Novel Virtual Reality-Based Haptic Simulator</t>
+  </si>
+  <si>
+    <t>Virtual reality haptic simulator</t>
+  </si>
+  <si>
+    <t>Results estimated from boxplot. Whole group data (subplot a) reported here.</t>
+  </si>
+  <si>
+    <t>Horeman et al.</t>
+  </si>
+  <si>
+    <t>Assessment of Laparoscopic Skills Based on Force and Motion Parameters</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Biomedical Engineering</t>
+  </si>
+  <si>
+    <t>Results estimated from boxplot, for task 2. Max force values used.</t>
+  </si>
+  <si>
+    <t>Trejos et al.</t>
+  </si>
+  <si>
+    <t>Development of force-based metrics for skills assessment in minimally invasive surgery</t>
+  </si>
+  <si>
+    <t>Simulated tumor removal and suturing</t>
+  </si>
+  <si>
+    <t>Used results for max grasp force, values evaluated from Fig. 4 (a). Compared experience level 1 and 6</t>
+  </si>
+  <si>
+    <t>Woodrow et al.</t>
+  </si>
+  <si>
+    <t>Training and evaluating spinal surgeons: The development of novel performance measures</t>
+  </si>
+  <si>
+    <t>Spine</t>
+  </si>
+  <si>
+    <t>Lumbar pedicle cannulation</t>
+  </si>
+  <si>
+    <t>Values estimated from Fig. 2. Values are mean forces. Compared results for lumbar level L2.</t>
+  </si>
+  <si>
+    <t>Sugiyama et al.</t>
+  </si>
+  <si>
+    <t>JAMA Surgery</t>
+  </si>
+  <si>
+    <t>Forces of Tool-Tissue Interaction to Assess Surgical Skill Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluated values from Fig. 3 c. Standardizer, maximum force. </t>
+  </si>
+  <si>
+    <t>Real neurosurgical procedures with various conditions</t>
+  </si>
+  <si>
+    <t>Shafiel et al.</t>
+  </si>
+  <si>
+    <t>Motor Skill Evaluation During Robot-Assisted Surgery</t>
+  </si>
+  <si>
+    <t>Volume 5A: 41st Mechanisms and Robotics Conference</t>
   </si>
 </sst>
 </file>
@@ -2633,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9C3E7-A606-4632-BFE8-84337DA69629}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,6 +2842,591 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFFA9462-4AD5-4A95-B8F1-A29FBB82FC76}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="A1:R1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H1" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>1.8</v>
+      </c>
+      <c r="K2">
+        <v>0.85</v>
+      </c>
+      <c r="L2">
+        <v>30</v>
+      </c>
+      <c r="M2">
+        <v>4.13</v>
+      </c>
+      <c r="N2">
+        <v>0.68</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>0.76970773674168036</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>-3.0271230088752055</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>-2.9878097230456575</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.37819168101706574</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBB5582-C584-406A-ABB8-AA0332D414F1}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H1" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>2015</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2">
+        <v>23</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>1*(3/4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="L2">
+        <v>19</v>
+      </c>
+      <c r="M2">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N2">
+        <f>0.5*(3/4)</f>
+        <v>0.375</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>0.61045577235373905</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>0.54604010385240109</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>0.53573746038348791</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.31568870931055087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" t="s">
+        <v>280</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <f>4*(3/4)</f>
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>25</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <f>2*(3/4)</f>
+        <v>1.5</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>2.3717082451262845</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <v>1.2649110640673518</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>1.2450433510191734</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.30983866769659335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4">
+        <v>2014</v>
+      </c>
+      <c r="D4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <f>4*(3/4)</f>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <v>2.5</v>
+      </c>
+      <c r="N4">
+        <f>3*(3/4)</f>
+        <v>2.25</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>2.6692695630078278</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <v>2.809757434745082</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>2.7081999371036933</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.58810470003328008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5">
+        <v>2014</v>
+      </c>
+      <c r="D5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>287</v>
+      </c>
+      <c r="H5" t="s">
+        <v>288</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>7.5</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>7.5166481891864541</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5" si="13">(J5-M5)/O5</f>
+        <v>1.6629752630943482</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>1.5350540890101676</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>0.66974767405542723</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6">
+        <v>2007</v>
+      </c>
+      <c r="D6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E6" t="s">
+        <v>291</v>
+      </c>
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>292</v>
+      </c>
+      <c r="H6" t="s">
+        <v>293</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>122</v>
+      </c>
+      <c r="K6">
+        <f>12*(3/4)</f>
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <v>88</v>
+      </c>
+      <c r="N6">
+        <f>10*(3/4)</f>
+        <v>7.5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O7" si="16">SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <v>8.5008650078890753</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P7" si="17">(J6-M6)/O6</f>
+        <v>3.9995929788847264</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q7" si="18">P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <v>3.8205067260988432</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R7" si="19">SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <v>0.80446095211216628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>298</v>
+      </c>
+      <c r="H7" t="s">
+        <v>297</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+      <c r="K7">
+        <f>2.9*(3/4)</f>
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>-0.1</v>
+      </c>
+      <c r="N7">
+        <f>1.5*(3/4)</f>
+        <v>1.125</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="16"/>
+        <v>1.7862320677896251</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="17"/>
+        <v>0.33590260236592362</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="18"/>
+        <v>0.30711095073455874</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="19"/>
+        <v>0.60975021804546647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7919254F-A5B3-4B18-98B0-711AB8CE8C49}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2767,7 +3436,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="B15" sqref="B15:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4240,10 +4909,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38582DD-83D6-42FC-BEAD-D85E565DA625}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4906,6 +5575,60 @@
       <c r="R11">
         <f t="shared" si="23"/>
         <v>0.75259275498598399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12">
+        <v>2017</v>
+      </c>
+      <c r="D12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F12" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12">
+        <v>717</v>
+      </c>
+      <c r="J12">
+        <v>599.13</v>
+      </c>
+      <c r="K12">
+        <v>881.81</v>
+      </c>
+      <c r="L12">
+        <v>413</v>
+      </c>
+      <c r="M12">
+        <v>271.37</v>
+      </c>
+      <c r="N12">
+        <v>578.65</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12" si="24">SQRT(((I12-1)*POWER(K12,2) + (L12-1)*POWER(N12,2))/((I12-1)+(L12-1)))</f>
+        <v>784.77647027401667</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12" si="25">(J12-M12)/O12</f>
+        <v>0.4176475880903483</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12" si="26">P12*(1- (3/(4*(I12+L12)-9)))</f>
+        <v>0.41736983531618049</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12" si="27">SQRT((I12+L12)/(I12*L12)+(POWER(P12,2)/(2*(I12+L12))))</f>
+        <v>6.2395423259094494E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6520,7 +7243,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="A4" sqref="A4:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Minor update to Author names.
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4F9368-9E72-408D-B6DC-FFDC41C05646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BE2787-758D-45B9-8A8A-43F41AFE22D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="311">
   <si>
     <t>Author</t>
   </si>
@@ -562,9 +562,6 @@
     <t>Effects and SDs estimated from barplots. Reported right hand movements</t>
   </si>
   <si>
-    <t>Goldbraikh</t>
-  </si>
-  <si>
     <t>Video-based fully automatic assessment of open surgery suturing skills</t>
   </si>
   <si>
@@ -733,9 +730,6 @@
     <t>Does not report idle time directly per skill group, only number of idle periods. Took values from the first segment, entering tissue with needle. Did not report SD for idle periods, estimated it from the SD of total operative time: SD_idle = M_idle*(SD_time/M_time).</t>
   </si>
   <si>
-    <t>Mackenzie</t>
-  </si>
-  <si>
     <t>Enhanced Training Benefits of Video Recording Surgery With Automated Hand Motion Analysis</t>
   </si>
   <si>
@@ -766,9 +760,6 @@
     <t>Values given as mean and 95% conf interval. SD calculated from conf interval by sqrt(N)*(upper lim - lower lim)/3.92. Results for non-dominant hand</t>
   </si>
   <si>
-    <t>Yamaguchi</t>
-  </si>
-  <si>
     <t>Objective assessment of laparoscopic suturing skills using a motion-tracking system</t>
   </si>
   <si>
@@ -983,6 +974,12 @@
   </si>
   <si>
     <t>Values given as medians. Sd estimated from boxplot</t>
+  </si>
+  <si>
+    <t>Mackenzie et al.</t>
+  </si>
+  <si>
+    <t>Goldbraikh et al.</t>
   </si>
 </sst>
 </file>
@@ -1302,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,13 +1328,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1468,19 +1465,19 @@
         <v>102.14</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O18" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O26" si="0">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>99.449960080434423</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P18" si="1">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P26" si="1">(J3-M3)/O3</f>
         <v>0.71895453695679024</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q18" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q26" si="2">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>0.70343753256203934</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R18" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R26" si="3">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.33937031474894647</v>
       </c>
     </row>
@@ -2344,7 +2341,7 @@
         <v>135</v>
       </c>
       <c r="H18" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I18">
         <v>4</v>
@@ -2427,19 +2424,19 @@
         <v>1083.75</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19" si="4">SQRT(((I19-1)*POWER(K19,2) + (L19-1)*POWER(N19,2))/((I19-1)+(L19-1)))</f>
+        <f t="shared" si="0"/>
         <v>1028.9793304532409</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19" si="5">(J19-M19)/O19</f>
+        <f t="shared" si="1"/>
         <v>0.19048001665268308</v>
       </c>
       <c r="Q19">
-        <f t="shared" ref="Q19" si="6">P19*(1- (3/(4*(I19+L19)-9)))</f>
+        <f t="shared" si="2"/>
         <v>0.18728761413895095</v>
       </c>
       <c r="R19">
-        <f t="shared" ref="R19" si="7">SQRT((I19+L19)/(I19*L19)+(POWER(P19,2)/(2*(I19+L19))))</f>
+        <f t="shared" si="3"/>
         <v>0.31955842537614054</v>
       </c>
     </row>
@@ -2448,13 +2445,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20">
         <v>2010</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
@@ -2463,7 +2460,7 @@
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -2484,19 +2481,19 @@
         <v>11.93</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O22" si="8">SQRT(((I20-1)*POWER(K20,2) + (L20-1)*POWER(N20,2))/((I20-1)+(L20-1)))</f>
+        <f t="shared" si="0"/>
         <v>12.581210527343277</v>
       </c>
       <c r="P20">
-        <f t="shared" ref="P20:P22" si="9">(J20-M20)/O20</f>
+        <f t="shared" si="1"/>
         <v>1.4259359193624681</v>
       </c>
       <c r="Q20">
-        <f t="shared" ref="Q20:Q22" si="10">P20*(1- (3/(4*(I20+L20)-9)))</f>
+        <f t="shared" si="2"/>
         <v>1.334918733020183</v>
       </c>
       <c r="R20">
-        <f t="shared" ref="R20:R22" si="11">SQRT((I20+L20)/(I20*L20)+(POWER(P20,2)/(2*(I20+L20))))</f>
+        <f t="shared" si="3"/>
         <v>0.60355967608829919</v>
       </c>
     </row>
@@ -2511,7 +2508,7 @@
         <v>2013</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -2520,7 +2517,7 @@
         <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I21">
         <v>11</v>
@@ -2542,19 +2539,19 @@
         <v>0.4</v>
       </c>
       <c r="O21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>1.7955674590502024</v>
       </c>
       <c r="P21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>1.4480102025101951</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>1.3790573357239952</v>
       </c>
       <c r="R21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.54037841581818158</v>
       </c>
     </row>
@@ -2563,25 +2560,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C22">
         <v>2018</v>
       </c>
       <c r="D22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" t="s">
         <v>233</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>234</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>235</v>
-      </c>
-      <c r="G22" t="s">
-        <v>236</v>
-      </c>
-      <c r="H22" t="s">
-        <v>237</v>
       </c>
       <c r="I22">
         <v>42</v>
@@ -2604,19 +2601,19 @@
         <v>6.5611332395977984</v>
       </c>
       <c r="O22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7.1930027137798414</v>
       </c>
       <c r="P22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>2.252188779098498</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>2.23417126886571</v>
       </c>
       <c r="R22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.26219564124906203</v>
       </c>
     </row>
@@ -2631,7 +2628,7 @@
         <v>2011</v>
       </c>
       <c r="D23" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -2643,7 +2640,7 @@
         <v>59</v>
       </c>
       <c r="H23" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -2664,19 +2661,19 @@
         <v>19</v>
       </c>
       <c r="O23">
-        <f t="shared" ref="O23" si="12">SQRT(((I23-1)*POWER(K23,2) + (L23-1)*POWER(N23,2))/((I23-1)+(L23-1)))</f>
+        <f t="shared" si="0"/>
         <v>20.554804791094465</v>
       </c>
       <c r="P23">
-        <f t="shared" ref="P23" si="13">(J23-M23)/O23</f>
+        <f t="shared" si="1"/>
         <v>4.8163921285641473</v>
       </c>
       <c r="Q23">
-        <f t="shared" ref="Q23" si="14">P23*(1- (3/(4*(I23+L23)-9)))</f>
+        <f t="shared" si="2"/>
         <v>4.587040122442045</v>
       </c>
       <c r="R23">
-        <f t="shared" ref="R23" si="15">SQRT((I23+L23)/(I23*L23)+(POWER(P23,2)/(2*(I23+L23))))</f>
+        <f t="shared" si="3"/>
         <v>0.93091402419722646</v>
       </c>
     </row>
@@ -2685,13 +2682,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24">
         <v>2009</v>
       </c>
       <c r="D24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E24" t="s">
         <v>158</v>
@@ -2700,10 +2697,10 @@
         <v>81</v>
       </c>
       <c r="G24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -2726,19 +2723,19 @@
         <v>50</v>
       </c>
       <c r="O24">
-        <f t="shared" ref="O24" si="16">SQRT(((I24-1)*POWER(K24,2) + (L24-1)*POWER(N24,2))/((I24-1)+(L24-1)))</f>
+        <f t="shared" si="0"/>
         <v>55.226805085936306</v>
       </c>
       <c r="P24">
-        <f t="shared" ref="P24" si="17">(J24-M24)/O24</f>
+        <f t="shared" si="1"/>
         <v>5.8848234927637044</v>
       </c>
       <c r="Q24">
-        <f t="shared" ref="Q24" si="18">P24*(1- (3/(4*(I24+L24)-9)))</f>
+        <f t="shared" si="2"/>
         <v>5.6361689789849567</v>
       </c>
       <c r="R24">
-        <f t="shared" ref="R24" si="19">SQRT((I24+L24)/(I24*L24)+(POWER(P24,2)/(2*(I24+L24))))</f>
+        <f t="shared" si="3"/>
         <v>1.0323655789131048</v>
       </c>
     </row>
@@ -2747,13 +2744,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C25">
         <v>2021</v>
       </c>
       <c r="D25" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
@@ -2765,7 +2762,7 @@
         <v>135</v>
       </c>
       <c r="H25" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -2786,19 +2783,19 @@
         <v>20.3</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O26" si="20">SQRT(((I25-1)*POWER(K25,2) + (L25-1)*POWER(N25,2))/((I25-1)+(L25-1)))</f>
+        <f t="shared" si="0"/>
         <v>23.412640053734101</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25:P26" si="21">(J25-M25)/O25</f>
+        <f t="shared" si="1"/>
         <v>0.57234040967809729</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25:Q26" si="22">P25*(1- (3/(4*(I25+L25)-9)))</f>
+        <f t="shared" si="2"/>
         <v>0.55998773896562037</v>
       </c>
       <c r="R25">
-        <f t="shared" ref="R25:R26" si="23">SQRT((I25+L25)/(I25*L25)+(POWER(P25,2)/(2*(I25+L25))))</f>
+        <f t="shared" si="3"/>
         <v>0.34544681474734895</v>
       </c>
     </row>
@@ -2807,13 +2804,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C26">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E26" t="s">
         <v>40</v>
@@ -2825,7 +2822,7 @@
         <v>135</v>
       </c>
       <c r="H26" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I26">
         <v>11</v>
@@ -2850,19 +2847,19 @@
         <v>30</v>
       </c>
       <c r="O26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="0"/>
         <v>89.472136209519093</v>
       </c>
       <c r="P26">
-        <f>(M26-J26)/O26</f>
-        <v>-1.021866418998546</v>
+        <f t="shared" si="1"/>
+        <v>1.021866418998546</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="22"/>
-        <v>-0.98099176223860418</v>
+        <f t="shared" si="2"/>
+        <v>0.98099176223860418</v>
       </c>
       <c r="R26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="3"/>
         <v>0.46451184813580504</v>
       </c>
     </row>
@@ -2876,10 +2873,13 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:R3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2898,13 +2898,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3366,19 +3366,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>310</v>
       </c>
       <c r="C9">
         <v>2021</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
         <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I9">
         <f>2*12</f>
@@ -3428,7 +3428,7 @@
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
@@ -3440,7 +3440,7 @@
         <v>159</v>
       </c>
       <c r="H10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I10">
         <f>(14/18)*135</f>
@@ -3483,13 +3483,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
@@ -3498,10 +3498,10 @@
         <v>41</v>
       </c>
       <c r="G11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" t="s">
         <v>178</v>
-      </c>
-      <c r="H11" t="s">
-        <v>179</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -3549,7 +3549,7 @@
         <v>2013</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -3558,7 +3558,7 @@
         <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I12">
         <v>11</v>
@@ -3628,13 +3628,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3761,13 +3761,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3823,7 +3823,7 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -3874,6 +3874,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3892,13 +3895,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3942,7 +3945,7 @@
         <v>2015</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -3951,10 +3954,10 @@
         <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I2">
         <v>23</v>
@@ -3999,13 +4002,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -4014,10 +4017,10 @@
         <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -4061,16 +4064,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C4">
         <v>2014</v>
       </c>
       <c r="D4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F4" t="s">
         <v>81</v>
@@ -4079,7 +4082,7 @@
         <v>135</v>
       </c>
       <c r="H4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -4123,13 +4126,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -4138,10 +4141,10 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -4183,25 +4186,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C6">
         <v>2007</v>
       </c>
       <c r="D6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F6" t="s">
         <v>151</v>
       </c>
       <c r="G6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -4245,25 +4248,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F7" t="s">
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -4324,10 +4327,13 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4346,13 +4352,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4491,19 +4497,19 @@
         <v>437.7</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O17" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>6351.4868544117062</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P17" si="5">(J3-M3)/O3</f>
         <v>1.3777514148394665</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q17" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>1.3160610529809829</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R17" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.54179548524236587</v>
       </c>
     </row>
@@ -4551,19 +4557,19 @@
         <v>117.3</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <f t="shared" si="4"/>
         <v>329.87375408838398</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <f t="shared" si="5"/>
         <v>2.7489304279631734</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <f t="shared" si="6"/>
         <v>2.6541397235506503</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <f t="shared" si="7"/>
         <v>0.57897092311695464</v>
       </c>
     </row>
@@ -4611,19 +4617,19 @@
         <v>23.47</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O6" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <f t="shared" si="4"/>
         <v>20.405207668632045</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P6" si="13">(J5-M5)/O5</f>
+        <f t="shared" si="5"/>
         <v>7.229527010733416</v>
       </c>
       <c r="Q5">
-        <f t="shared" ref="Q5:Q6" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <f t="shared" si="6"/>
         <v>6.2865452267247095</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R6" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <f t="shared" si="7"/>
         <v>1.9407804615496191</v>
       </c>
     </row>
@@ -4632,19 +4638,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>310</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
         <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -4665,19 +4671,19 @@
         <v>1250</v>
       </c>
       <c r="O6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>1951.5618744994995</v>
       </c>
       <c r="P6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>2.0496403687051155</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>2.0174470644846165</v>
       </c>
       <c r="R6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0.34948313484124172</v>
       </c>
     </row>
@@ -4686,13 +4692,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7">
         <v>2017</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
@@ -4704,7 +4710,7 @@
         <v>125</v>
       </c>
       <c r="H7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I7">
         <v>24</v>
@@ -4727,19 +4733,19 @@
         <v>3000</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7" si="16">SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <f t="shared" si="4"/>
         <v>5632.7649108178248</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7" si="17">(J7-M7)/O7</f>
+        <f t="shared" si="5"/>
         <v>0.88766353277009868</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7" si="18">P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.86954795046866806</v>
       </c>
       <c r="R7">
-        <f t="shared" ref="R7" si="19">SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <f t="shared" si="7"/>
         <v>0.34414417348878751</v>
       </c>
     </row>
@@ -4754,7 +4760,7 @@
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -4763,7 +4769,7 @@
         <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -4785,19 +4791,19 @@
         <v>0.5</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8" si="20">SQRT(((I8-1)*POWER(K8,2) + (L8-1)*POWER(N8,2))/((I8-1)+(L8-1)))</f>
+        <f t="shared" si="4"/>
         <v>2.980404754391591</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8" si="21">(J8-M8)/O8</f>
+        <f t="shared" si="5"/>
         <v>0.83881224398004317</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8" si="22">P8*(1- (3/(4*(I8+L8)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.79886880379051728</v>
       </c>
       <c r="R8">
-        <f t="shared" ref="R8" si="23">SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
+        <f t="shared" si="7"/>
         <v>0.50329995463924693</v>
       </c>
     </row>
@@ -4806,25 +4812,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" t="s">
         <v>202</v>
-      </c>
-      <c r="E9" t="s">
-        <v>203</v>
       </c>
       <c r="F9" t="s">
         <v>81</v>
       </c>
       <c r="G9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H9" t="s">
         <v>204</v>
-      </c>
-      <c r="H9" t="s">
-        <v>205</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -4847,19 +4853,19 @@
         <v>600</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O10" si="24">SQRT(((I9-1)*POWER(K9,2) + (L9-1)*POWER(N9,2))/((I9-1)+(L9-1)))</f>
+        <f t="shared" si="4"/>
         <v>663.08936049374222</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:P10" si="25">(J9-M9)/O9</f>
+        <f t="shared" si="5"/>
         <v>0.30161847243496448</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:Q10" si="26">P9*(1- (3/(4*(I9+L9)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.2888740299377125</v>
       </c>
       <c r="R9">
-        <f t="shared" ref="R9:R10" si="27">SQRT((I9+L9)/(I9*L9)+(POWER(P9,2)/(2*(I9+L9))))</f>
+        <f t="shared" si="7"/>
         <v>0.5610475403857057</v>
       </c>
     </row>
@@ -4868,13 +4874,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10">
         <v>2009</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" t="s">
         <v>158</v>
@@ -4883,10 +4889,10 @@
         <v>41</v>
       </c>
       <c r="G10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" t="s">
         <v>208</v>
-      </c>
-      <c r="H10" t="s">
-        <v>209</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -4909,19 +4915,19 @@
         <v>300</v>
       </c>
       <c r="O10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="4"/>
         <v>571.18298293979308</v>
       </c>
       <c r="P10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="5"/>
         <v>2.1884405476620428</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="26"/>
+        <f t="shared" si="6"/>
         <v>2.0959712287467451</v>
       </c>
       <c r="R10">
-        <f t="shared" si="27"/>
+        <f t="shared" si="7"/>
         <v>0.565448318386644</v>
       </c>
     </row>
@@ -4930,22 +4936,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11">
         <v>2015</v>
       </c>
       <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" t="s">
         <v>224</v>
-      </c>
-      <c r="E11" t="s">
-        <v>225</v>
       </c>
       <c r="F11" t="s">
         <v>151</v>
       </c>
       <c r="G11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -4966,19 +4972,19 @@
         <v>1.29</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O14" si="28">SQRT(((I11-1)*POWER(K11,2) + (L11-1)*POWER(N11,2))/((I11-1)+(L11-1)))</f>
+        <f t="shared" si="4"/>
         <v>1.29</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11:P14" si="29">(J11-M11)/O11</f>
+        <f t="shared" si="5"/>
         <v>1.9147286821705425</v>
       </c>
       <c r="Q11">
-        <f t="shared" ref="Q11:Q14" si="30">P11*(1- (3/(4*(I11+L11)-9)))</f>
+        <f t="shared" si="6"/>
         <v>1.7506090808416388</v>
       </c>
       <c r="R11">
-        <f t="shared" ref="R11:R14" si="31">SQRT((I11+L11)/(I11*L11)+(POWER(P11,2)/(2*(I11+L11))))</f>
+        <f t="shared" si="7"/>
         <v>0.73028178225921214</v>
       </c>
     </row>
@@ -4987,25 +4993,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" t="s">
         <v>233</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>234</v>
       </c>
-      <c r="F12" t="s">
-        <v>235</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>236</v>
-      </c>
-      <c r="H12" t="s">
-        <v>238</v>
       </c>
       <c r="I12">
         <v>42</v>
@@ -5028,19 +5034,19 @@
         <v>5.2489065916782387</v>
       </c>
       <c r="O12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="4"/>
         <v>5.5663659820625027</v>
       </c>
       <c r="P12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="5"/>
         <v>1.8144692664023596</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
         <v>1.7999535122711408</v>
       </c>
       <c r="R12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="7"/>
         <v>0.24387585261365186</v>
       </c>
     </row>
@@ -5055,7 +5061,7 @@
         <v>2016</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
@@ -5067,7 +5073,7 @@
         <v>159</v>
       </c>
       <c r="H13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I13">
         <f>(14/18)*135</f>
@@ -5089,19 +5095,19 @@
         <v>0.1</v>
       </c>
       <c r="O13">
-        <f t="shared" si="28"/>
+        <f t="shared" si="4"/>
         <v>0.22594829403858613</v>
       </c>
       <c r="P13">
-        <f t="shared" si="29"/>
+        <f t="shared" si="5"/>
         <v>2.4341852295909536</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
         <v>2.4204327706667113</v>
       </c>
       <c r="R13">
-        <f t="shared" si="31"/>
+        <f t="shared" si="7"/>
         <v>0.25456343387139785</v>
       </c>
     </row>
@@ -5110,13 +5116,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>167</v>
       </c>
       <c r="C14">
         <v>2011</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -5128,7 +5134,7 @@
         <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I14">
         <v>9</v>
@@ -5149,19 +5155,19 @@
         <v>220</v>
       </c>
       <c r="O14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="4"/>
         <v>268.21726268083489</v>
       </c>
       <c r="P14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="5"/>
         <v>3.5344481206195608</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="6"/>
         <v>3.3661410672567245</v>
       </c>
       <c r="R14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="7"/>
         <v>0.75447412733327679</v>
       </c>
     </row>
@@ -5176,7 +5182,7 @@
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -5185,10 +5191,10 @@
         <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I15">
         <v>23</v>
@@ -5211,19 +5217,19 @@
         <v>225</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15:O17" si="32">SQRT(((I15-1)*POWER(K15,2) + (L15-1)*POWER(N15,2))/((I15-1)+(L15-1)))</f>
+        <f t="shared" si="4"/>
         <v>576.32998360314377</v>
       </c>
       <c r="P15">
-        <f t="shared" ref="P15:P17" si="33">(J15-M15)/O15</f>
+        <f t="shared" si="5"/>
         <v>1.0410702498052837</v>
       </c>
       <c r="Q15">
-        <f t="shared" ref="Q15:Q17" si="34">P15*(1- (3/(4*(I15+L15)-9)))</f>
+        <f t="shared" si="6"/>
         <v>1.0214274149032974</v>
       </c>
       <c r="R15">
-        <f t="shared" ref="R15:R17" si="35">SQRT((I15+L15)/(I15*L15)+(POWER(P15,2)/(2*(I15+L15))))</f>
+        <f t="shared" si="7"/>
         <v>0.33017047922702103</v>
       </c>
     </row>
@@ -5232,13 +5238,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -5247,10 +5253,10 @@
         <v>81</v>
       </c>
       <c r="G16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -5273,19 +5279,19 @@
         <v>0.89999999999999947</v>
       </c>
       <c r="O16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>4.0868396181543671</v>
       </c>
       <c r="P16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>0.92981383050115773</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="6"/>
         <v>0.90713544439137339</v>
       </c>
       <c r="R16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.36786073670199965</v>
       </c>
     </row>
@@ -5294,13 +5300,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C17">
         <v>2010</v>
       </c>
       <c r="D17" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -5312,7 +5318,7 @@
         <v>135</v>
       </c>
       <c r="H17" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I17">
         <v>11</v>
@@ -5335,19 +5341,19 @@
         <v>0.75</v>
       </c>
       <c r="O17">
-        <f t="shared" si="32"/>
+        <f t="shared" si="4"/>
         <v>0.79494933451412142</v>
       </c>
       <c r="P17">
-        <f t="shared" si="33"/>
+        <f t="shared" si="5"/>
         <v>1.257941804066302</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="34"/>
+        <f t="shared" si="6"/>
         <v>1.2076241319036498</v>
       </c>
       <c r="R17">
-        <f t="shared" si="35"/>
+        <f t="shared" si="7"/>
         <v>0.47810636893297231</v>
       </c>
     </row>
@@ -5361,10 +5367,13 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5383,13 +5392,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5445,7 +5454,7 @@
         <v>125</v>
       </c>
       <c r="H2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -5489,13 +5498,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3">
         <v>2015</v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
         <v>91</v>
@@ -5507,7 +5516,7 @@
         <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -5528,19 +5537,19 @@
         <v>1.48</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <f t="shared" ref="O3:O8" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
         <v>7.0231563417027818</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <f t="shared" ref="P3:P8" si="5">(J3-M3)/O3</f>
         <v>1.7485015856877082</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <f t="shared" ref="Q3:Q8" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
         <v>1.6932857461396753</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <f t="shared" ref="R3:R8" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
         <v>0.46515500288968653</v>
       </c>
     </row>
@@ -5549,25 +5558,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4">
         <v>2015</v>
       </c>
       <c r="D4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" t="s">
         <v>224</v>
-      </c>
-      <c r="E4" t="s">
-        <v>225</v>
       </c>
       <c r="F4" t="s">
         <v>151</v>
       </c>
       <c r="G4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" t="s">
         <v>226</v>
-      </c>
-      <c r="H4" t="s">
-        <v>227</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -5590,19 +5599,19 @@
         <v>9.8676330345222194</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <f t="shared" si="4"/>
         <v>11.542321913112083</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <f t="shared" si="5"/>
         <v>3.0323188231511704</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <f t="shared" si="6"/>
         <v>2.7724057811667842</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <f t="shared" si="7"/>
         <v>0.88578737731681323</v>
       </c>
     </row>
@@ -5611,13 +5620,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>309</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E5" t="s">
         <v>158</v>
@@ -5626,10 +5635,10 @@
         <v>151</v>
       </c>
       <c r="G5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -5652,19 +5661,19 @@
         <v>0.24560260586319216</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <f t="shared" si="4"/>
         <v>3.4514275412635569</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5" si="13">(J5-M5)/O5</f>
+        <f t="shared" si="5"/>
         <v>0.63741740879618369</v>
       </c>
       <c r="Q5">
-        <f t="shared" ref="Q5" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.36423851931210494</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <f t="shared" si="7"/>
         <v>1.0250793233352993</v>
       </c>
     </row>
@@ -5673,25 +5682,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>2013</v>
       </c>
       <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" t="s">
         <v>202</v>
-      </c>
-      <c r="E6" t="s">
-        <v>203</v>
       </c>
       <c r="F6" t="s">
         <v>81</v>
       </c>
       <c r="G6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H6" t="s">
         <v>204</v>
-      </c>
-      <c r="H6" t="s">
-        <v>205</v>
       </c>
       <c r="I6">
         <v>16</v>
@@ -5714,19 +5723,19 @@
         <v>7.5</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6" si="16">SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <f t="shared" si="4"/>
         <v>14.031215200402281</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6" si="17">(J6-M6)/O6</f>
+        <f t="shared" si="5"/>
         <v>0.99777530313971763</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6" si="18">P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.95561578328874375</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6" si="19">SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <f t="shared" si="7"/>
         <v>0.5808518648406743</v>
       </c>
     </row>
@@ -5735,25 +5744,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" t="s">
         <v>233</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>234</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>235</v>
-      </c>
-      <c r="G7" t="s">
-        <v>236</v>
-      </c>
-      <c r="H7" t="s">
-        <v>237</v>
       </c>
       <c r="I7">
         <v>42</v>
@@ -5776,19 +5785,19 @@
         <v>108.72735082762065</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7" si="20">SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <f t="shared" si="4"/>
         <v>427.1486564213152</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7" si="21">(J7-M7)/O7</f>
+        <f t="shared" si="5"/>
         <v>0.70467270697232554</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7" si="22">P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.69903532531654688</v>
       </c>
       <c r="R7">
-        <f t="shared" ref="R7" si="23">SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <f t="shared" si="7"/>
         <v>0.21192996768458866</v>
       </c>
     </row>
@@ -5797,25 +5806,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" t="s">
         <v>264</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>265</v>
-      </c>
-      <c r="F8" t="s">
-        <v>266</v>
-      </c>
-      <c r="G8" t="s">
-        <v>267</v>
-      </c>
-      <c r="H8" t="s">
-        <v>268</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -5836,19 +5845,19 @@
         <v>10.25</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8" si="24">SQRT(((I8-1)*POWER(K8,2) + (L8-1)*POWER(N8,2))/((I8-1)+(L8-1)))</f>
+        <f t="shared" si="4"/>
         <v>13.73753448935266</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8" si="25">(J8-M8)/O8</f>
+        <f t="shared" si="5"/>
         <v>0.65441145985604265</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8" si="26">P8*(1- (3/(4*(I8+L8)-9)))</f>
+        <f t="shared" si="6"/>
         <v>0.61591666809980483</v>
       </c>
       <c r="R8">
-        <f t="shared" ref="R8" si="27">SQRT((I8+L8)/(I8*L8)+(POWER(P8,2)/(2*(I8+L8))))</f>
+        <f t="shared" si="7"/>
         <v>0.56060248420162262</v>
       </c>
     </row>
@@ -5861,11 +5870,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38582DD-83D6-42FC-BEAD-D85E565DA625}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5884,13 +5896,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5928,13 +5940,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -5943,10 +5955,10 @@
         <v>75</v>
       </c>
       <c r="G2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" t="s">
         <v>185</v>
-      </c>
-      <c r="H2" t="s">
-        <v>186</v>
       </c>
       <c r="I2">
         <v>36</v>
@@ -5988,13 +6000,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3">
         <v>2006</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -6045,13 +6057,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -6060,10 +6072,10 @@
         <v>81</v>
       </c>
       <c r="G4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" t="s">
         <v>191</v>
-      </c>
-      <c r="H4" t="s">
-        <v>192</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6107,16 +6119,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
         <v>194</v>
-      </c>
-      <c r="E5" t="s">
-        <v>195</v>
       </c>
       <c r="F5" t="s">
         <v>151</v>
@@ -6125,7 +6137,7 @@
         <v>125</v>
       </c>
       <c r="H5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I5">
         <v>22</v>
@@ -6169,13 +6181,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -6184,10 +6196,10 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" t="s">
         <v>199</v>
-      </c>
-      <c r="H6" t="s">
-        <v>200</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -6229,25 +6241,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>2013</v>
       </c>
       <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
         <v>202</v>
-      </c>
-      <c r="E7" t="s">
-        <v>203</v>
       </c>
       <c r="F7" t="s">
         <v>81</v>
       </c>
       <c r="G7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H7" t="s">
         <v>204</v>
-      </c>
-      <c r="H7" t="s">
-        <v>205</v>
       </c>
       <c r="I7">
         <v>16</v>
@@ -6289,13 +6301,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -6304,7 +6316,7 @@
         <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I8">
         <v>13</v>
@@ -6346,25 +6358,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" t="s">
         <v>214</v>
-      </c>
-      <c r="E9" t="s">
-        <v>215</v>
       </c>
       <c r="F9" t="s">
         <v>140</v>
       </c>
       <c r="G9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H9" t="s">
         <v>216</v>
-      </c>
-      <c r="H9" t="s">
-        <v>217</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -6426,7 +6438,7 @@
         <v>104</v>
       </c>
       <c r="H10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I10">
         <v>32</v>
@@ -6485,10 +6497,10 @@
         <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I11">
         <v>28</v>
@@ -6532,16 +6544,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F12" t="s">
         <v>140</v>
@@ -6586,13 +6598,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -6604,7 +6616,7 @@
         <v>135</v>
       </c>
       <c r="H13" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -6652,11 +6664,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E75FBFA-590A-44E1-B3FD-3060EE11E94F}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -6675,13 +6690,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -6719,25 +6734,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
         <v>194</v>
-      </c>
-      <c r="E2" t="s">
-        <v>195</v>
       </c>
       <c r="F2" t="s">
         <v>151</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -6760,19 +6775,19 @@
         <v>141.06971830985918</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O6" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <f t="shared" ref="O2:O5" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
         <v>212.45602112623581</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P6" si="1">(J2-M2)/O2</f>
+        <f t="shared" ref="P2:P5" si="1">(J2-M2)/O2</f>
         <v>-0.38873927677920322</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q6" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <f t="shared" ref="Q2:Q5" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
         <v>-0.37133304050550753</v>
       </c>
       <c r="R2">
-        <f t="shared" ref="R2:R6" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <f t="shared" ref="R2:R5" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
         <v>0.46377570711932226</v>
       </c>
     </row>
@@ -6781,19 +6796,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I3">
         <v>21</v>
@@ -6835,13 +6850,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -6850,10 +6865,10 @@
         <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6897,13 +6912,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
@@ -6912,10 +6927,10 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I5">
         <v>14</v>
@@ -6957,13 +6972,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -6972,10 +6987,10 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -7028,6 +7043,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7046,13 +7064,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7090,13 +7108,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -7105,10 +7123,10 @@
         <v>75</v>
       </c>
       <c r="G2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" t="s">
         <v>199</v>
-      </c>
-      <c r="H2" t="s">
-        <v>200</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -7150,13 +7168,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -7165,10 +7183,10 @@
         <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I3">
         <v>14</v>
@@ -7210,13 +7228,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4">
         <v>2006</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -7267,13 +7285,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -7282,10 +7300,10 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I5">
         <v>15</v>
@@ -7329,13 +7347,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
@@ -7347,7 +7365,7 @@
         <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -7406,10 +7424,10 @@
         <v>140</v>
       </c>
       <c r="G7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I7">
         <f>5*3</f>
@@ -7459,7 +7477,7 @@
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -7468,7 +7486,7 @@
         <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -7512,19 +7530,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I9">
         <v>21</v>
@@ -7566,25 +7584,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
         <v>194</v>
-      </c>
-      <c r="E10" t="s">
-        <v>195</v>
       </c>
       <c r="F10" t="s">
         <v>151</v>
       </c>
       <c r="G10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -7646,7 +7664,7 @@
         <v>135</v>
       </c>
       <c r="H11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -7715,13 +7733,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7884,10 +7902,13 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7906,13 +7927,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8244,25 +8265,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -8316,6 +8337,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8334,13 +8358,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added sample size plot
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BE2787-758D-45B9-8A8A-43F41AFE22D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAD03AB-99DE-4253-809E-DC511B34C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="309">
   <si>
     <t>Author</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Journal of Surgical Education</t>
   </si>
   <si>
-    <t>microscope</t>
-  </si>
-  <si>
     <t>effects estimated from boxplot</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Surgical Endoscopy</t>
   </si>
   <si>
-    <t>robotic</t>
-  </si>
-  <si>
     <t>suture tying</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
     <t>Microsurgery</t>
   </si>
   <si>
-    <t>Microscope</t>
-  </si>
-  <si>
     <t>Needle piercing in VR</t>
   </si>
   <si>
@@ -980,6 +971,9 @@
   </si>
   <si>
     <t>Goldbraikh et al.</t>
+  </si>
+  <si>
+    <t>Robotic Surgery</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1294,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,13 +1322,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1384,7 +1378,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1441,7 +1435,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1498,13 +1492,13 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>23</v>
@@ -1560,13 +1554,13 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5">
         <f>(14/18)*135</f>
@@ -1609,25 +1603,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>2009</v>
       </c>
       <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>308</v>
+      </c>
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
       </c>
       <c r="I6">
         <v>15</v>
@@ -1669,25 +1663,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>2002</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>43</v>
       </c>
       <c r="I7">
         <v>15</v>
@@ -1729,25 +1723,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>2002</v>
       </c>
       <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" t="s">
-        <v>48</v>
       </c>
       <c r="I8">
         <v>20</v>
@@ -1789,22 +1783,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>2004</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9">
         <v>13</v>
@@ -1846,25 +1840,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>2008</v>
       </c>
       <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
         <v>53</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -1906,25 +1900,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>2009</v>
       </c>
       <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
         <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" t="s">
-        <v>60</v>
       </c>
       <c r="I11">
         <v>13</v>
@@ -1966,25 +1960,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12">
         <v>2020</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
       </c>
       <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
       </c>
       <c r="I12">
         <v>26</v>
@@ -2026,22 +2020,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13">
         <v>2004</v>
       </c>
       <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
         <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>69</v>
       </c>
       <c r="I13">
         <v>25</v>
@@ -2083,25 +2077,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>2010</v>
       </c>
       <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
         <v>74</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" t="s">
-        <v>78</v>
       </c>
       <c r="I14">
         <v>7</v>
@@ -2143,25 +2137,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>1999</v>
       </c>
       <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" t="s">
         <v>79</v>
       </c>
-      <c r="E15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>81</v>
-      </c>
-      <c r="G15" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" t="s">
-        <v>84</v>
       </c>
       <c r="I15">
         <v>8</v>
@@ -2203,25 +2197,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" t="s">
         <v>133</v>
-      </c>
-      <c r="E16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" t="s">
-        <v>136</v>
       </c>
       <c r="I16">
         <v>12</v>
@@ -2263,25 +2257,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C17">
         <v>2001</v>
       </c>
       <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
         <v>149</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" t="s">
-        <v>151</v>
-      </c>
-      <c r="G17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" t="s">
-        <v>152</v>
       </c>
       <c r="I17">
         <v>12</v>
@@ -2323,25 +2317,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C18">
         <v>2012</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I18">
         <v>4</v>
@@ -2383,25 +2377,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C19">
         <v>2007</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I19">
         <v>14</v>
@@ -2445,22 +2439,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C20">
         <v>2010</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -2502,22 +2496,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>2013</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I21">
         <v>11</v>
@@ -2560,25 +2554,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C22">
         <v>2018</v>
       </c>
       <c r="D22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" t="s">
+        <v>230</v>
+      </c>
+      <c r="G22" t="s">
         <v>231</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
         <v>232</v>
-      </c>
-      <c r="F22" t="s">
-        <v>233</v>
-      </c>
-      <c r="G22" t="s">
-        <v>234</v>
-      </c>
-      <c r="H22" t="s">
-        <v>235</v>
       </c>
       <c r="I22">
         <v>42</v>
@@ -2622,25 +2616,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C23">
         <v>2011</v>
       </c>
       <c r="D23" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -2682,25 +2676,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C24">
         <v>2009</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -2744,25 +2738,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C25">
         <v>2021</v>
       </c>
       <c r="D25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H25" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -2804,25 +2798,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C26">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I26">
         <v>11</v>
@@ -2872,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2027-C5D7-4FCE-B720-F07DC782C0FB}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2898,13 +2892,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2942,25 +2936,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2">
         <v>2001</v>
       </c>
       <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
         <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" t="s">
-        <v>152</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -3002,25 +2996,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -3068,19 +3062,19 @@
         <v>2022</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4">
         <v>30</v>
@@ -3122,25 +3116,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C5">
         <v>2003</v>
       </c>
       <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" t="s">
         <v>157</v>
-      </c>
-      <c r="E5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" t="s">
-        <v>160</v>
       </c>
       <c r="I5">
         <v>16</v>
@@ -3184,25 +3178,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>2002</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>15</v>
@@ -3244,25 +3238,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C7">
         <v>2007</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I7">
         <v>14</v>
@@ -3306,25 +3300,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C8">
         <v>2007</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -3366,19 +3360,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C9">
         <v>2021</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I9">
         <f>2*12</f>
@@ -3428,19 +3422,19 @@
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I10">
         <f>(14/18)*135</f>
@@ -3483,25 +3477,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -3543,22 +3537,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C12">
         <v>2013</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I12">
         <v>11</v>
@@ -3628,13 +3622,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3672,25 +3666,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" t="s">
         <v>137</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
         <v>139</v>
-      </c>
-      <c r="F2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" t="s">
-        <v>142</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -3761,13 +3755,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3811,19 +3805,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -3895,13 +3889,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3945,19 +3939,19 @@
         <v>2015</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I2">
         <v>23</v>
@@ -4002,25 +3996,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -4064,25 +4058,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C4">
         <v>2014</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -4126,25 +4120,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -4186,25 +4180,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C6">
         <v>2007</v>
       </c>
       <c r="D6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" t="s">
+        <v>286</v>
+      </c>
+      <c r="H6" t="s">
         <v>287</v>
-      </c>
-      <c r="E6" t="s">
-        <v>288</v>
-      </c>
-      <c r="F6" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H6" t="s">
-        <v>290</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -4248,25 +4242,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
         <v>292</v>
       </c>
-      <c r="F7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" t="s">
-        <v>295</v>
-      </c>
       <c r="H7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -4327,7 +4321,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4352,13 +4346,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4396,25 +4390,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C2">
         <v>2007</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I2">
         <v>14</v>
@@ -4458,25 +4452,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>2004</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I3">
         <v>13</v>
@@ -4518,25 +4512,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>2002</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -4578,25 +4572,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -4638,19 +4632,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -4692,25 +4689,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7">
         <v>2017</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I7">
         <v>24</v>
@@ -4754,22 +4751,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -4812,25 +4809,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
         <v>201</v>
-      </c>
-      <c r="E9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" t="s">
-        <v>203</v>
-      </c>
-      <c r="H9" t="s">
-        <v>204</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -4874,25 +4871,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C10">
         <v>2009</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -4936,22 +4933,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C11">
         <v>2015</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -4993,25 +4990,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" t="s">
+        <v>230</v>
+      </c>
+      <c r="G12" t="s">
         <v>231</v>
       </c>
-      <c r="E12" t="s">
-        <v>232</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>233</v>
-      </c>
-      <c r="G12" t="s">
-        <v>234</v>
-      </c>
-      <c r="H12" t="s">
-        <v>236</v>
       </c>
       <c r="I12">
         <v>42</v>
@@ -5061,19 +5058,19 @@
         <v>2016</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I13">
         <f>(14/18)*135</f>
@@ -5116,25 +5113,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C14">
         <v>2011</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I14">
         <v>9</v>
@@ -5182,19 +5179,19 @@
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I15">
         <v>23</v>
@@ -5238,25 +5235,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H16" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -5300,25 +5297,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C17">
         <v>2010</v>
       </c>
       <c r="D17" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H17" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I17">
         <v>11</v>
@@ -5392,13 +5389,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5442,19 +5439,19 @@
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -5498,25 +5495,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C3">
         <v>2015</v>
       </c>
       <c r="D3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" t="s">
         <v>218</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" t="s">
-        <v>221</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -5558,25 +5555,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C4">
         <v>2015</v>
       </c>
       <c r="D4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" t="s">
         <v>223</v>
-      </c>
-      <c r="E4" t="s">
-        <v>224</v>
-      </c>
-      <c r="F4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H4" t="s">
-        <v>226</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -5620,25 +5617,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -5682,25 +5679,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6">
         <v>2013</v>
       </c>
       <c r="D6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H6" t="s">
         <v>201</v>
-      </c>
-      <c r="E6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H6" t="s">
-        <v>204</v>
       </c>
       <c r="I6">
         <v>16</v>
@@ -5744,25 +5741,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" t="s">
         <v>231</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>232</v>
-      </c>
-      <c r="F7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H7" t="s">
-        <v>235</v>
       </c>
       <c r="I7">
         <v>42</v>
@@ -5806,25 +5803,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G8" t="s">
         <v>261</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>262</v>
-      </c>
-      <c r="F8" t="s">
-        <v>263</v>
-      </c>
-      <c r="G8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H8" t="s">
-        <v>265</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -5870,7 +5867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38582DD-83D6-42FC-BEAD-D85E565DA625}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -5896,13 +5893,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5940,25 +5937,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C2">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I2">
         <v>36</v>
@@ -6000,22 +5997,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C3">
         <v>2006</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -6057,25 +6054,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6119,25 +6116,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C5">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I5">
         <v>22</v>
@@ -6181,25 +6178,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -6241,25 +6238,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C7">
         <v>2013</v>
       </c>
       <c r="D7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" t="s">
         <v>201</v>
-      </c>
-      <c r="E7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" t="s">
-        <v>204</v>
       </c>
       <c r="I7">
         <v>16</v>
@@ -6301,22 +6298,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I8">
         <v>13</v>
@@ -6358,25 +6355,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H9" t="s">
         <v>213</v>
-      </c>
-      <c r="E9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F9" t="s">
-        <v>140</v>
-      </c>
-      <c r="G9" t="s">
-        <v>215</v>
-      </c>
-      <c r="H9" t="s">
-        <v>216</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -6420,25 +6417,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I10">
         <v>32</v>
@@ -6482,25 +6479,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I11">
         <v>28</v>
@@ -6544,19 +6541,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I12">
         <v>717</v>
@@ -6598,25 +6595,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H13" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -6690,13 +6687,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -6734,25 +6731,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -6796,19 +6793,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I3">
         <v>21</v>
@@ -6850,25 +6847,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6912,25 +6909,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I5">
         <v>14</v>
@@ -6972,25 +6969,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -7039,7 +7036,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7064,13 +7061,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7108,25 +7105,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -7168,25 +7165,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I3">
         <v>14</v>
@@ -7228,22 +7225,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>2006</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -7285,25 +7282,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I5">
         <v>15</v>
@@ -7347,25 +7344,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -7409,25 +7406,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>2009</v>
       </c>
       <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
       <c r="F7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I7">
         <f>5*3</f>
@@ -7471,22 +7468,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -7530,19 +7527,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I9">
         <v>21</v>
@@ -7584,25 +7581,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -7646,25 +7643,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -7733,13 +7730,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7783,19 +7780,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -7837,25 +7834,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>1996</v>
       </c>
       <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>88</v>
-      </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -7902,7 +7899,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7927,13 +7924,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7977,19 +7974,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -8032,25 +8029,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>2017</v>
       </c>
       <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
         <v>94</v>
-      </c>
-      <c r="E3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" t="s">
-        <v>97</v>
       </c>
       <c r="I3">
         <v>28</v>
@@ -8092,19 +8089,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>2022</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -8146,25 +8143,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>2016</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" t="s">
         <v>102</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" t="s">
-        <v>105</v>
       </c>
       <c r="I5">
         <v>32</v>
@@ -8208,22 +8205,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I6">
         <v>8</v>
@@ -8265,25 +8262,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
         <v>244</v>
       </c>
-      <c r="E7" t="s">
-        <v>246</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>247</v>
-      </c>
       <c r="H7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -8358,13 +8355,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8402,25 +8399,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
         <v>111</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>112</v>
-      </c>
-      <c r="F2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" t="s">
-        <v>115</v>
       </c>
       <c r="I2">
         <f>50*20</f>
@@ -8464,25 +8461,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3">
         <v>2019</v>
       </c>
       <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
         <v>117</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>118</v>
-      </c>
-      <c r="F3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
       </c>
       <c r="I3">
         <v>13</v>
@@ -8524,25 +8521,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" t="s">
         <v>123</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" t="s">
-        <v>126</v>
       </c>
       <c r="I4">
         <v>50</v>
@@ -8585,25 +8582,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
         <v>128</v>
-      </c>
-      <c r="E5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" t="s">
-        <v>131</v>
       </c>
       <c r="I5">
         <v>7</v>
@@ -8645,25 +8642,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C6">
         <v>2020</v>
       </c>
       <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" t="s">
         <v>137</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
         <v>139</v>
-      </c>
-      <c r="F6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -8707,25 +8704,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" t="s">
         <v>144</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" t="s">
-        <v>147</v>
       </c>
       <c r="I7">
         <v>12</v>

</xml_diff>

<commit_message>
Added OSATS results and removed grasp results for now.
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAD03AB-99DE-4253-809E-DC511B34C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECCDC8D-C2D7-402D-B3A9-E4CE4CAB2D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="336">
   <si>
     <t>Author</t>
   </si>
@@ -974,6 +974,87 @@
   </si>
   <si>
     <t>Robotic Surgery</t>
+  </si>
+  <si>
+    <t>Nickel et al.</t>
+  </si>
+  <si>
+    <t>Direct Observation versus Endoscopic Video Recording-Based Rating with the Objective Structured Assessment of Technical Skills for Training of Laparoscopic Cholecystectomy</t>
+  </si>
+  <si>
+    <t>European Surgical Research</t>
+  </si>
+  <si>
+    <t>OSATS score from Table 1, direct observation, novices and experts compared</t>
+  </si>
+  <si>
+    <t>Paley et al.</t>
+  </si>
+  <si>
+    <t>Crowdsourced Assessment of Surgical Skill Proficiency in Cataract Surgery</t>
+  </si>
+  <si>
+    <t>Used modified OSATS. SD estimated from Figure 1F. Used expert ratings.</t>
+  </si>
+  <si>
+    <t>Kassab et al.</t>
+  </si>
+  <si>
+    <t>"Blowing up the barriers" in surgical training: Exploring and validating the concept of distributed simulation</t>
+  </si>
+  <si>
+    <t>Study had two tasks, results are for DS (distributed simulation) because these results were given in the text (box trainer results only as figure). Note that DS was novel task developed for this study.</t>
+  </si>
+  <si>
+    <t>Black et al.</t>
+  </si>
+  <si>
+    <t>Assessment of surgical competence at carotid endarterectomy under local anaesthesia in a simulated operating theatre</t>
+  </si>
+  <si>
+    <t>British Journal of Surgery</t>
+  </si>
+  <si>
+    <t>Results for crisis scenario</t>
+  </si>
+  <si>
+    <t>Willems et al.</t>
+  </si>
+  <si>
+    <t>Assessing Endovascular Skills using the Simulator for Testing and Rating Endovascular Skills (STRESS) Machine</t>
+  </si>
+  <si>
+    <t>European Journal of Vascular and Endovascular Surgery</t>
+  </si>
+  <si>
+    <t>Combination of OSATS and some other score? May not be suitable for comparison here. Remove in the future. SDs estimated from Figure 2.</t>
+  </si>
+  <si>
+    <t>Leong et al.</t>
+  </si>
+  <si>
+    <t>Validation of orthopaedic bench models for trauma surgery</t>
+  </si>
+  <si>
+    <t>Journal of Bone and Joint Surgery - Series B</t>
+  </si>
+  <si>
+    <t>Used results for DCP, dynamic comperssion plate. Esimtaed values from boxplot.</t>
+  </si>
+  <si>
+    <t>Hance et al.</t>
+  </si>
+  <si>
+    <t>Objective assessment of technical skills in cardiac surgery</t>
+  </si>
+  <si>
+    <t>European Journal of Cardio-thoracic Surgery</t>
+  </si>
+  <si>
+    <t>LAD anastomosis</t>
+  </si>
+  <si>
+    <t>Paper reported several tasks, live and blinded scoring. Values here are for LAD anastomosis, blinded scoring.</t>
   </si>
 </sst>
 </file>
@@ -2866,7 +2947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2027-C5D7-4FCE-B720-F07DC782C0FB}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3600,7 +3681,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="A1:R1"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4306,12 +4387,468 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7919254F-A5B3-4B18-98B0-711AB8CE8C49}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2">
+        <v>2016</v>
+      </c>
+      <c r="D2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>48.6</v>
+      </c>
+      <c r="K2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>65.3</v>
+      </c>
+      <c r="N2">
+        <v>10.4</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="0">SQRT(((I2-1)*POWER(K2,2) + (L2-1)*POWER(N2,2))/((I2-1)+(L2-1)))</f>
+        <v>9.2479300671185758</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2" si="1">(J2-M2)/O2</f>
+        <v>-1.8058095031857544</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2" si="2">P2*(1- (3/(4*(I2+L2)-9)))</f>
+        <v>-1.7335771230583241</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2" si="3">SQRT((I2+L2)/(I2*L2)+(POWER(P2,2)/(2*(I2+L2))))</f>
+        <v>0.55765128124243823</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>7.3</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>21</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3" si="4">SQRT(((I3-1)*POWER(K3,2) + (L3-1)*POWER(N3,2))/((I3-1)+(L3-1)))</f>
+        <v>3.3741095691478935</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3" si="5">(J3-M3)/O3</f>
+        <v>-4.0603305017921612</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3" si="6">P3*(1- (3/(4*(I3+L3)-9)))</f>
+        <v>-3.8214875310985046</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3" si="7">SQRT((I3+L3)/(I3*L3)+(POWER(P3,2)/(2*(I3+L3))))</f>
+        <v>0.9095716412523922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4">
+        <v>2011</v>
+      </c>
+      <c r="D4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" t="s">
+        <v>318</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>16.3</v>
+      </c>
+      <c r="K4">
+        <v>3.8</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>27.3</v>
+      </c>
+      <c r="N4">
+        <v>5.7</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4" si="8">SQRT(((I4-1)*POWER(K4,2) + (L4-1)*POWER(N4,2))/((I4-1)+(L4-1)))</f>
+        <v>4.8440685379131452</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4" si="9">(J4-M4)/O4</f>
+        <v>-2.2708184068631838</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4" si="10">P4*(1- (3/(4*(I4+L4)-9)))</f>
+        <v>-2.1748683333337535</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4" si="11">SQRT((I4+L4)/(I4*L4)+(POWER(P4,2)/(2*(I4+L4))))</f>
+        <v>0.5735114697403324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5">
+        <v>2010</v>
+      </c>
+      <c r="D5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" t="s">
+        <v>321</v>
+      </c>
+      <c r="H5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>15.5</v>
+      </c>
+      <c r="K5">
+        <f>(19-12)*(3/4)</f>
+        <v>5.25</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>36</v>
+      </c>
+      <c r="N5">
+        <f>(36-35)*(3/4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5" si="12">SQRT(((I5-1)*POWER(K5,2) + (L5-1)*POWER(N5,2))/((I5-1)+(L5-1)))</f>
+        <v>3.75</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5" si="13">(J5-M5)/O5</f>
+        <v>-5.4666666666666668</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5" si="14">P5*(1- (3/(4*(I5+L5)-9)))</f>
+        <v>-5.2356807511737093</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5" si="15">SQRT((I5+L5)/(I5*L5)+(POWER(P5,2)/(2*(I5+L5))))</f>
+        <v>0.97319633739092493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6">
+        <v>2009</v>
+      </c>
+      <c r="D6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6" t="s">
+        <v>325</v>
+      </c>
+      <c r="H6" t="s">
+        <v>326</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>42.75</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>82.8</v>
+      </c>
+      <c r="N6">
+        <f>25*(3/5)</f>
+        <v>15</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="16">SQRT(((I6-1)*POWER(K6,2) + (L6-1)*POWER(N6,2))/((I6-1)+(L6-1)))</f>
+        <v>9.8857105322416121</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6" si="17">(J6-M6)/O6</f>
+        <v>-4.0513021162595733</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6" si="18">P6*(1- (3/(4*(I6+L6)-9)))</f>
+        <v>-3.7686531314042542</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6" si="19">SQRT((I6+L6)/(I6*L6)+(POWER(P6,2)/(2*(I6+L6))))</f>
+        <v>0.977891154026579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7">
+        <v>2008</v>
+      </c>
+      <c r="D7" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" t="s">
+        <v>329</v>
+      </c>
+      <c r="H7" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <f>15*(3/4)</f>
+        <v>11.25</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>65</v>
+      </c>
+      <c r="N7">
+        <f>12*(3/4)</f>
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O8" si="20">SQRT(((I7-1)*POWER(K7,2) + (L7-1)*POWER(N7,2))/((I7-1)+(L7-1)))</f>
+        <v>10.371987514454498</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:P8" si="21">(J7-M7)/O7</f>
+        <v>-2.892406104248749</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q8" si="22">P7*(1- (3/(4*(I7+L7)-9)))</f>
+        <v>-2.7077844380201057</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R8" si="23">SQRT((I7+L7)/(I7*L7)+(POWER(P7,2)/(2*(I7+L7))))</f>
+        <v>0.768409297058403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8">
+        <v>2005</v>
+      </c>
+      <c r="D8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E8" t="s">
+        <v>333</v>
+      </c>
+      <c r="G8" t="s">
+        <v>334</v>
+      </c>
+      <c r="H8" t="s">
+        <v>335</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>15.5</v>
+      </c>
+      <c r="K8">
+        <f>(19.5-13.25)*(3/4)</f>
+        <v>4.6875</v>
+      </c>
+      <c r="L8">
+        <v>13</v>
+      </c>
+      <c r="M8">
+        <v>24</v>
+      </c>
+      <c r="N8">
+        <f>(34-21)*(3/4)</f>
+        <v>9.75</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="20"/>
+        <v>7.752837401347918</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="21"/>
+        <v>-1.0963727935945335</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="22"/>
+        <v>-1.0602286355639445</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="23"/>
+        <v>0.42929835348752027</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Included notes to the printout of table of studies
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C686B-EC6C-4D6A-B1F4-35665A470AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4487EA-D47A-43C2-BF2A-CC8EB6633383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="345">
   <si>
     <t>Author</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>Optimizing Assessment of Surgical Knot Tying Skill</t>
-  </si>
-  <si>
-    <t>General</t>
   </si>
   <si>
     <t>knot tying</t>
@@ -1405,7 +1402,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1433,13 +1430,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1489,7 +1486,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1546,7 +1543,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1603,7 +1600,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -1665,7 +1662,7 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -1726,7 +1723,7 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
@@ -1786,7 +1783,7 @@
         <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -1846,7 +1843,7 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
         <v>45</v>
@@ -1906,7 +1903,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
         <v>49</v>
@@ -1963,7 +1960,7 @@
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -2023,7 +2020,7 @@
         <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -2083,13 +2080,13 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" t="s">
         <v>61</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>62</v>
-      </c>
-      <c r="H12" t="s">
-        <v>63</v>
       </c>
       <c r="I12">
         <v>26</v>
@@ -2131,22 +2128,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13">
         <v>2004</v>
       </c>
       <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" t="s">
         <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" t="s">
-        <v>67</v>
       </c>
       <c r="I13">
         <v>25</v>
@@ -2188,25 +2185,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>2010</v>
       </c>
       <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
         <v>72</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>74</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
       </c>
       <c r="I14">
         <v>7</v>
@@ -2248,25 +2245,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15">
         <v>1999</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" t="s">
         <v>80</v>
-      </c>
-      <c r="F15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" t="s">
-        <v>81</v>
       </c>
       <c r="I15">
         <v>8</v>
@@ -2308,25 +2305,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
         <v>130</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" t="s">
         <v>131</v>
       </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>132</v>
-      </c>
-      <c r="H16" t="s">
-        <v>133</v>
       </c>
       <c r="I16">
         <v>12</v>
@@ -2368,25 +2365,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17">
         <v>2001</v>
       </c>
       <c r="D17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" t="s">
         <v>146</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>147</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
         <v>148</v>
-      </c>
-      <c r="G17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" t="s">
-        <v>149</v>
       </c>
       <c r="I17">
         <v>12</v>
@@ -2428,25 +2425,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18">
         <v>2012</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I18">
         <v>4</v>
@@ -2488,25 +2485,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19">
         <v>2007</v>
       </c>
       <c r="D19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" t="s">
         <v>161</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" t="s">
         <v>162</v>
-      </c>
-      <c r="F19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" t="s">
-        <v>158</v>
-      </c>
-      <c r="H19" t="s">
-        <v>163</v>
       </c>
       <c r="I19">
         <v>14</v>
@@ -2550,22 +2547,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20">
         <v>2010</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -2607,22 +2604,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21">
         <v>2013</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I21">
         <v>11</v>
@@ -2665,25 +2662,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C22">
         <v>2018</v>
       </c>
       <c r="D22" t="s">
+        <v>227</v>
+      </c>
+      <c r="E22" t="s">
         <v>228</v>
       </c>
-      <c r="E22" t="s">
-        <v>229</v>
-      </c>
       <c r="F22" t="s">
+        <v>307</v>
+      </c>
+      <c r="G22" t="s">
         <v>230</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>231</v>
-      </c>
-      <c r="H22" t="s">
-        <v>232</v>
       </c>
       <c r="I22">
         <v>42</v>
@@ -2727,25 +2724,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23">
         <v>2011</v>
       </c>
       <c r="D23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
         <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -2787,25 +2784,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24">
         <v>2009</v>
       </c>
       <c r="D24" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
         <v>203</v>
       </c>
-      <c r="E24" t="s">
-        <v>155</v>
-      </c>
-      <c r="F24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" t="s">
-        <v>204</v>
-      </c>
       <c r="H24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -2849,25 +2846,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C25">
         <v>2021</v>
       </c>
       <c r="D25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -2909,25 +2906,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C26">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I26">
         <v>11</v>
@@ -3003,13 +3000,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3047,25 +3044,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2">
         <v>2001</v>
       </c>
       <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" t="s">
         <v>146</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>147</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>148</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>149</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -3107,25 +3104,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" t="s">
         <v>151</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" t="s">
-        <v>152</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -3173,19 +3170,19 @@
         <v>2022</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4">
         <v>30</v>
@@ -3227,25 +3224,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5">
         <v>2003</v>
       </c>
       <c r="D5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" t="s">
         <v>154</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" t="s">
         <v>155</v>
       </c>
-      <c r="F5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>156</v>
-      </c>
-      <c r="H5" t="s">
-        <v>157</v>
       </c>
       <c r="I5">
         <v>16</v>
@@ -3301,13 +3298,13 @@
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" t="s">
         <v>158</v>
-      </c>
-      <c r="H6" t="s">
-        <v>159</v>
       </c>
       <c r="I6">
         <v>15</v>
@@ -3349,25 +3346,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>2007</v>
       </c>
       <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
         <v>161</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" t="s">
         <v>162</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
-        <v>158</v>
-      </c>
-      <c r="H7" t="s">
-        <v>163</v>
       </c>
       <c r="I7">
         <v>14</v>
@@ -3411,25 +3408,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8">
         <v>2007</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" t="s">
         <v>166</v>
-      </c>
-      <c r="H8" t="s">
-        <v>167</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -3471,19 +3468,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C9">
         <v>2021</v>
       </c>
       <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" t="s">
         <v>168</v>
-      </c>
-      <c r="E9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" t="s">
-        <v>169</v>
       </c>
       <c r="I9">
         <f>2*12</f>
@@ -3533,19 +3530,19 @@
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I10">
         <f>(14/18)*135</f>
@@ -3588,25 +3585,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" t="s">
         <v>174</v>
-      </c>
-      <c r="H11" t="s">
-        <v>175</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -3648,22 +3645,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12">
         <v>2013</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I12">
         <v>11</v>
@@ -3733,13 +3730,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3777,25 +3774,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
         <v>136</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>137</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>138</v>
-      </c>
-      <c r="H2" t="s">
-        <v>139</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -3839,25 +3836,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
         <v>337</v>
       </c>
-      <c r="E3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>338</v>
-      </c>
-      <c r="H3" t="s">
-        <v>339</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -3928,13 +3925,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3978,19 +3975,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -4062,13 +4059,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4112,19 +4109,19 @@
         <v>2015</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I2">
         <v>23</v>
@@ -4169,25 +4166,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" t="s">
         <v>273</v>
-      </c>
-      <c r="H3" t="s">
-        <v>274</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -4231,25 +4228,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C4">
         <v>2014</v>
       </c>
       <c r="D4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" t="s">
         <v>276</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" t="s">
         <v>277</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" t="s">
-        <v>278</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -4293,25 +4290,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
+        <v>280</v>
+      </c>
+      <c r="H5" t="s">
         <v>281</v>
-      </c>
-      <c r="H5" t="s">
-        <v>282</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -4353,25 +4350,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6">
         <v>2007</v>
       </c>
       <c r="D6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" t="s">
         <v>284</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" t="s">
         <v>285</v>
       </c>
-      <c r="F6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>286</v>
-      </c>
-      <c r="H6" t="s">
-        <v>287</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -4415,25 +4412,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>289</v>
+      </c>
+      <c r="E7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H7" t="s">
         <v>290</v>
-      </c>
-      <c r="E7" t="s">
-        <v>289</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>292</v>
-      </c>
-      <c r="H7" t="s">
-        <v>291</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -4477,19 +4474,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C8">
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I8">
         <v>8</v>
@@ -4560,13 +4557,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4604,22 +4601,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" t="s">
         <v>310</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
         <v>311</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" t="s">
-        <v>312</v>
       </c>
       <c r="I2">
         <v>15</v>
@@ -4661,19 +4658,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I3">
         <v>6</v>
@@ -4715,25 +4712,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C4">
         <v>2011</v>
       </c>
       <c r="D4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" t="s">
         <v>317</v>
-      </c>
-      <c r="E4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" t="s">
-        <v>318</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -4775,19 +4772,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C5">
         <v>2010</v>
       </c>
       <c r="D5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5" t="s">
         <v>320</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>321</v>
-      </c>
-      <c r="H5" t="s">
-        <v>322</v>
       </c>
       <c r="I5">
         <v>10</v>
@@ -4831,19 +4828,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C6">
         <v>2009</v>
       </c>
       <c r="D6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" t="s">
         <v>324</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>325</v>
-      </c>
-      <c r="H6" t="s">
-        <v>326</v>
       </c>
       <c r="I6">
         <v>8</v>
@@ -4886,19 +4883,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C7">
         <v>2008</v>
       </c>
       <c r="D7" t="s">
+        <v>327</v>
+      </c>
+      <c r="E7" t="s">
         <v>328</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>329</v>
-      </c>
-      <c r="H7" t="s">
-        <v>330</v>
       </c>
       <c r="I7">
         <v>8</v>
@@ -4942,22 +4939,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8" t="s">
         <v>332</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>333</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>334</v>
-      </c>
-      <c r="H8" t="s">
-        <v>335</v>
       </c>
       <c r="I8">
         <v>12</v>
@@ -5001,25 +4998,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
+        <v>337</v>
+      </c>
+      <c r="H9" t="s">
         <v>341</v>
-      </c>
-      <c r="E9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" t="s">
-        <v>338</v>
-      </c>
-      <c r="H9" t="s">
-        <v>342</v>
       </c>
       <c r="I9">
         <v>22</v>
@@ -5093,13 +5090,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5137,25 +5134,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2">
         <v>2007</v>
       </c>
       <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
         <v>161</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" t="s">
         <v>162</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" t="s">
-        <v>163</v>
       </c>
       <c r="I2">
         <v>14</v>
@@ -5211,7 +5208,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
         <v>39</v>
@@ -5271,13 +5268,13 @@
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" t="s">
         <v>158</v>
-      </c>
-      <c r="H4" t="s">
-        <v>159</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -5319,25 +5316,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" t="s">
         <v>151</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H5" t="s">
-        <v>152</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -5379,22 +5376,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" t="s">
         <v>168</v>
-      </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" t="s">
-        <v>169</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -5436,25 +5433,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7">
         <v>2017</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I7">
         <v>24</v>
@@ -5498,22 +5495,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -5556,25 +5553,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
         <v>198</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
         <v>199</v>
       </c>
-      <c r="F9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>200</v>
-      </c>
-      <c r="H9" t="s">
-        <v>201</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -5618,25 +5615,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10">
         <v>2009</v>
       </c>
       <c r="D10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s">
         <v>203</v>
       </c>
-      <c r="E10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>204</v>
-      </c>
-      <c r="H10" t="s">
-        <v>205</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -5680,22 +5677,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11">
         <v>2015</v>
       </c>
       <c r="D11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" t="s">
         <v>220</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" t="s">
         <v>221</v>
-      </c>
-      <c r="F11" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" t="s">
-        <v>222</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -5737,25 +5734,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" t="s">
         <v>228</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>229</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>230</v>
       </c>
-      <c r="G12" t="s">
-        <v>231</v>
-      </c>
       <c r="H12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I12">
         <v>42</v>
@@ -5805,19 +5802,19 @@
         <v>2016</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I13">
         <f>(14/18)*135</f>
@@ -5860,25 +5857,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14">
         <v>2011</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I14">
         <v>9</v>
@@ -5926,19 +5923,19 @@
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
+        <v>237</v>
+      </c>
+      <c r="H15" t="s">
         <v>238</v>
-      </c>
-      <c r="H15" t="s">
-        <v>239</v>
       </c>
       <c r="I15">
         <v>23</v>
@@ -5982,25 +5979,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -6044,25 +6041,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C17">
         <v>2010</v>
       </c>
       <c r="D17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E17" t="s">
         <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I17">
         <v>11</v>
@@ -6136,13 +6133,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -6186,19 +6183,19 @@
         <v>2021</v>
       </c>
       <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -6242,25 +6239,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3">
         <v>2015</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -6302,25 +6299,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4">
         <v>2015</v>
       </c>
       <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" t="s">
         <v>220</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" t="s">
         <v>221</v>
       </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>222</v>
-      </c>
-      <c r="H4" t="s">
-        <v>223</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -6364,25 +6361,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" t="s">
         <v>224</v>
       </c>
-      <c r="E5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>225</v>
-      </c>
-      <c r="H5" t="s">
-        <v>226</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -6426,25 +6423,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6">
         <v>2013</v>
       </c>
       <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" t="s">
         <v>198</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" t="s">
         <v>199</v>
       </c>
-      <c r="F6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>200</v>
-      </c>
-      <c r="H6" t="s">
-        <v>201</v>
       </c>
       <c r="I6">
         <v>16</v>
@@ -6488,25 +6485,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" t="s">
         <v>228</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>229</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>230</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>231</v>
-      </c>
-      <c r="H7" t="s">
-        <v>232</v>
       </c>
       <c r="I7">
         <v>42</v>
@@ -6550,25 +6547,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" t="s">
         <v>258</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>259</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>260</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>261</v>
-      </c>
-      <c r="H8" t="s">
-        <v>262</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -6640,13 +6637,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -6684,25 +6681,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" t="s">
         <v>181</v>
-      </c>
-      <c r="H2" t="s">
-        <v>182</v>
       </c>
       <c r="I2">
         <v>36</v>
@@ -6744,22 +6741,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3">
         <v>2006</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -6801,25 +6798,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" t="s">
         <v>187</v>
-      </c>
-      <c r="H4" t="s">
-        <v>188</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6863,25 +6860,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
         <v>190</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" t="s">
         <v>191</v>
-      </c>
-      <c r="F5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" t="s">
-        <v>192</v>
       </c>
       <c r="I5">
         <v>22</v>
@@ -6925,25 +6922,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" t="s">
         <v>195</v>
-      </c>
-      <c r="H6" t="s">
-        <v>196</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -6985,25 +6982,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7">
         <v>2013</v>
       </c>
       <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" t="s">
         <v>198</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
         <v>199</v>
       </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>200</v>
-      </c>
-      <c r="H7" t="s">
-        <v>201</v>
       </c>
       <c r="I7">
         <v>16</v>
@@ -7045,22 +7042,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I8">
         <v>13</v>
@@ -7102,25 +7099,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" t="s">
         <v>210</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" t="s">
         <v>211</v>
       </c>
-      <c r="F9" t="s">
-        <v>137</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>212</v>
-      </c>
-      <c r="H9" t="s">
-        <v>213</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -7164,25 +7161,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I10">
         <v>32</v>
@@ -7226,25 +7223,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
         <v>91</v>
       </c>
-      <c r="E11" t="s">
-        <v>92</v>
-      </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
+        <v>266</v>
+      </c>
+      <c r="H11" t="s">
         <v>267</v>
-      </c>
-      <c r="H11" t="s">
-        <v>268</v>
       </c>
       <c r="I11">
         <v>28</v>
@@ -7288,19 +7285,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
+        <v>293</v>
+      </c>
+      <c r="E12" t="s">
         <v>294</v>
       </c>
-      <c r="E12" t="s">
-        <v>295</v>
-      </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I12">
         <v>717</v>
@@ -7342,25 +7339,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -7434,13 +7431,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7478,25 +7475,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
         <v>190</v>
       </c>
-      <c r="E2" t="s">
-        <v>191</v>
-      </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2" t="s">
         <v>296</v>
-      </c>
-      <c r="H2" t="s">
-        <v>297</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -7540,19 +7537,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
         <v>254</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>255</v>
-      </c>
-      <c r="H3" t="s">
-        <v>256</v>
       </c>
       <c r="I3">
         <v>21</v>
@@ -7594,25 +7591,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -7656,25 +7653,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I5">
         <v>14</v>
@@ -7716,25 +7713,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -7808,13 +7805,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7852,25 +7849,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" t="s">
         <v>195</v>
-      </c>
-      <c r="H2" t="s">
-        <v>196</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -7912,25 +7909,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3" t="s">
         <v>248</v>
-      </c>
-      <c r="H3" t="s">
-        <v>249</v>
       </c>
       <c r="I3">
         <v>14</v>
@@ -7972,22 +7969,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4">
         <v>2006</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -8029,25 +8026,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I5">
         <v>15</v>
@@ -8091,25 +8088,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -8165,13 +8162,13 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" t="s">
         <v>251</v>
-      </c>
-      <c r="H7" t="s">
-        <v>252</v>
       </c>
       <c r="I7">
         <f>5*3</f>
@@ -8215,22 +8212,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -8274,19 +8271,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" t="s">
         <v>254</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>255</v>
-      </c>
-      <c r="H9" t="s">
-        <v>256</v>
       </c>
       <c r="I9">
         <v>21</v>
@@ -8328,25 +8325,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" t="s">
         <v>190</v>
       </c>
-      <c r="E10" t="s">
-        <v>191</v>
-      </c>
       <c r="F10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H10" t="s">
         <v>296</v>
-      </c>
-      <c r="H10" t="s">
-        <v>297</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -8390,25 +8387,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -8477,13 +8474,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8527,19 +8524,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -8581,25 +8578,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>1996</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>86</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -8671,13 +8668,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8721,19 +8718,19 @@
         <v>2022</v>
       </c>
       <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -8776,25 +8773,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3">
         <v>2017</v>
       </c>
       <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>93</v>
-      </c>
-      <c r="H3" t="s">
-        <v>94</v>
       </c>
       <c r="I3">
         <v>28</v>
@@ -8836,19 +8833,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>2022</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -8890,25 +8887,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>2016</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
         <v>101</v>
-      </c>
-      <c r="H5" t="s">
-        <v>102</v>
       </c>
       <c r="I5">
         <v>32</v>
@@ -8952,22 +8949,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" t="s">
         <v>105</v>
-      </c>
-      <c r="H6" t="s">
-        <v>106</v>
       </c>
       <c r="I6">
         <v>8</v>
@@ -9009,25 +9006,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
         <v>243</v>
       </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>244</v>
-      </c>
-      <c r="H7" t="s">
-        <v>245</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -9102,13 +9099,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
         <v>264</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>265</v>
-      </c>
-      <c r="H1" t="s">
-        <v>266</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -9146,25 +9143,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>110</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>111</v>
-      </c>
-      <c r="H2" t="s">
-        <v>112</v>
       </c>
       <c r="I2">
         <f>50*20</f>
@@ -9208,25 +9205,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3">
         <v>2019</v>
       </c>
       <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
         <v>114</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>115</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>116</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>117</v>
-      </c>
-      <c r="H3" t="s">
-        <v>118</v>
       </c>
       <c r="I3">
         <v>13</v>
@@ -9268,25 +9265,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
         <v>120</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
         <v>121</v>
       </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>122</v>
-      </c>
-      <c r="H4" t="s">
-        <v>123</v>
       </c>
       <c r="I4">
         <v>50</v>
@@ -9329,25 +9326,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
         <v>125</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
         <v>126</v>
       </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>127</v>
-      </c>
-      <c r="H5" t="s">
-        <v>128</v>
       </c>
       <c r="I5">
         <v>7</v>
@@ -9389,25 +9386,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6">
         <v>2020</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
         <v>136</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>137</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>138</v>
-      </c>
-      <c r="H6" t="s">
-        <v>139</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -9451,25 +9448,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
         <v>142</v>
       </c>
-      <c r="E7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>143</v>
-      </c>
-      <c r="H7" t="s">
-        <v>144</v>
       </c>
       <c r="I7">
         <v>12</v>
@@ -9511,25 +9508,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E8" t="s">
+        <v>320</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" t="s">
         <v>337</v>
       </c>
-      <c r="E8" t="s">
-        <v>321</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>338</v>
-      </c>
-      <c r="H8" t="s">
-        <v>339</v>
       </c>
       <c r="I8">
         <v>2</v>

</xml_diff>

<commit_message>
Added summary metrics to the intro from all studies
</commit_message>
<xml_diff>
--- a/data/surgical_metrics.xlsx
+++ b/data/surgical_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankos\tyokansio\projektit\meta-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C23BA5-8742-4C59-A363-AD6680B9C24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49311482-35E7-475F-AE08-3DEF9A4C404D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_time" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="410">
   <si>
     <t>Author</t>
   </si>
@@ -392,9 +392,6 @@
     <t>Clinical Simulation in Nursing</t>
   </si>
   <si>
-    <t>Various nursing tasks</t>
-  </si>
-  <si>
     <t>Elevate HOB</t>
   </si>
   <si>
@@ -446,18 +443,12 @@
     <t>Transporting and loading task</t>
   </si>
   <si>
-    <t>Visual behaviour in robotic surgery—Demonstrating the validity of the simulated environment</t>
-  </si>
-  <si>
     <t>Dilley et al.</t>
   </si>
   <si>
     <t>International Journal of Medical Robotics and Computer Assisted Surgery</t>
   </si>
   <si>
-    <t>Robotic surgery</t>
-  </si>
-  <si>
     <t>Fundamentals of Robotic Surgery, simulator task</t>
   </si>
   <si>
@@ -488,9 +479,6 @@
     <t>Journal of the American College of Surgeons</t>
   </si>
   <si>
-    <t>Open surgery</t>
-  </si>
-  <si>
     <t>Used ICSAD system to record data. Several skill groups, here we compare basic surgical trainees and consultants</t>
   </si>
   <si>
@@ -548,9 +536,6 @@
     <t>Effects and SDs estimated from barplots. Reported right hand movements</t>
   </si>
   <si>
-    <t>Video-based fully automatic assessment of open surgery suturing skills</t>
-  </si>
-  <si>
     <t>Task:Balloon dominant hand</t>
   </si>
   <si>
@@ -1284,6 +1269,15 @@
   </si>
   <si>
     <t>Idle time values from Table 2, given as percentage. Note, idle time defined as time when "no reaction between instruments and the tissue was measured."</t>
+  </si>
+  <si>
+    <t>Visual behaviour in Robotic Surgery—Demonstrating the validity of the simulated environment</t>
+  </si>
+  <si>
+    <t>Open Surgery</t>
+  </si>
+  <si>
+    <t>Video-based fully automatic assessment of Open Surgery suturing skills</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1598,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,13 +1626,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1864,7 +1858,7 @@
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -1925,7 +1919,7 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
@@ -1985,7 +1979,7 @@
         <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -2045,7 +2039,7 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
         <v>45</v>
@@ -2105,7 +2099,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G9" t="s">
         <v>49</v>
@@ -2162,7 +2156,7 @@
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -2222,7 +2216,7 @@
         <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
@@ -2282,7 +2276,7 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G12" t="s">
         <v>61</v>
@@ -2342,7 +2336,7 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
         <v>66</v>
@@ -2459,7 +2453,7 @@
         <v>78</v>
       </c>
       <c r="F15" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G15" t="s">
         <v>77</v>
@@ -2507,25 +2501,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" t="s">
         <v>128</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" t="s">
         <v>129</v>
       </c>
-      <c r="F16" t="s">
-        <v>258</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>130</v>
-      </c>
-      <c r="H16" t="s">
-        <v>131</v>
       </c>
       <c r="I16">
         <v>12</v>
@@ -2567,25 +2561,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C17">
         <v>2001</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G17" t="s">
         <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I17">
         <v>12</v>
@@ -2627,25 +2621,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C18">
         <v>2012</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
         <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I18">
         <v>4</v>
@@ -2687,25 +2681,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C19">
         <v>2007</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F19" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I19">
         <v>14</v>
@@ -2749,22 +2743,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C20">
         <v>2010</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -2812,16 +2806,16 @@
         <v>2013</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E21" t="s">
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H21" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I21">
         <v>11</v>
@@ -2864,25 +2858,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C22">
         <v>2018</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F22" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G22" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H22" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I22">
         <v>42</v>
@@ -2926,25 +2920,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C23">
         <v>2011</v>
       </c>
       <c r="D23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G23" t="s">
         <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -2986,25 +2980,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C24">
         <v>2009</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F24" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G24" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -3048,25 +3042,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C25">
         <v>2021</v>
       </c>
       <c r="D25" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -3108,25 +3102,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C26">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H26" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I26">
         <v>11</v>
@@ -3172,25 +3166,25 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C27">
         <v>2014</v>
       </c>
       <c r="D27" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I27">
         <v>11</v>
@@ -3232,25 +3226,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C28">
         <v>2021</v>
       </c>
       <c r="D28" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E28" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H28" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I28">
         <v>2</v>
@@ -3294,25 +3288,25 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C29">
         <v>2016</v>
       </c>
       <c r="D29" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E29" t="s">
         <v>86</v>
       </c>
       <c r="F29" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G29" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H29" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="I29">
         <v>6</v>
@@ -3356,25 +3350,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C30">
         <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E30" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F30" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G30" t="s">
         <v>83</v>
       </c>
       <c r="H30" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I30">
         <f>30*2</f>
@@ -3418,16 +3412,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C31">
         <v>2022</v>
       </c>
       <c r="D31" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E31" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F31" t="s">
         <v>72</v>
@@ -3436,7 +3430,7 @@
         <v>77</v>
       </c>
       <c r="H31" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I31">
         <v>10</v>
@@ -3480,25 +3474,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C32">
         <v>2021</v>
       </c>
       <c r="D32" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E32" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F32" t="s">
         <v>72</v>
       </c>
       <c r="G32" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H32" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I32">
         <v>9</v>
@@ -3540,25 +3534,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C33">
         <v>2022</v>
       </c>
       <c r="D33" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E33" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="F33" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G33" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H33" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I33">
         <f>13*9</f>
@@ -3602,25 +3596,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C34">
         <v>2006</v>
       </c>
       <c r="D34" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E34" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F34" t="s">
         <v>72</v>
       </c>
       <c r="G34" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="H34" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I34">
         <v>10</v>
@@ -3664,25 +3658,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C35">
         <v>2019</v>
       </c>
       <c r="D35" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E35" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F35" t="s">
         <v>72</v>
       </c>
       <c r="G35" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H35" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I35">
         <v>20</v>
@@ -3724,25 +3718,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C36">
         <v>2020</v>
       </c>
       <c r="D36" t="s">
+        <v>403</v>
+      </c>
+      <c r="E36" t="s">
+        <v>381</v>
+      </c>
+      <c r="F36" t="s">
         <v>408</v>
       </c>
-      <c r="E36" t="s">
-        <v>386</v>
-      </c>
-      <c r="F36" t="s">
-        <v>146</v>
-      </c>
       <c r="G36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H36" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="I36">
         <v>11</v>
@@ -3788,8 +3782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298FF69-1A01-44B7-9B68-125032E688E1}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3814,13 +3808,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3932,13 +3926,13 @@
         <v>113</v>
       </c>
       <c r="F3" t="s">
+        <v>408</v>
+      </c>
+      <c r="G3" t="s">
         <v>114</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>115</v>
-      </c>
-      <c r="H3" t="s">
-        <v>116</v>
       </c>
       <c r="I3">
         <v>13</v>
@@ -3980,25 +3974,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
         <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>119</v>
       </c>
       <c r="F4" t="s">
         <v>72</v>
       </c>
       <c r="G4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" t="s">
         <v>120</v>
-      </c>
-      <c r="H4" t="s">
-        <v>121</v>
       </c>
       <c r="I4">
         <v>50</v>
@@ -4041,25 +4035,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
         <v>123</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" t="s">
         <v>124</v>
       </c>
-      <c r="F5" t="s">
-        <v>258</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>125</v>
-      </c>
-      <c r="H5" t="s">
-        <v>126</v>
       </c>
       <c r="I5">
         <v>7</v>
@@ -4101,25 +4095,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C6">
         <v>2020</v>
       </c>
       <c r="D6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E6" t="s">
         <v>132</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" t="s">
         <v>134</v>
-      </c>
-      <c r="F6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" t="s">
-        <v>137</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -4163,25 +4157,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" t="s">
         <v>139</v>
-      </c>
-      <c r="F7" t="s">
-        <v>258</v>
-      </c>
-      <c r="G7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" t="s">
-        <v>142</v>
       </c>
       <c r="I7">
         <v>12</v>
@@ -4223,25 +4217,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H8" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -4312,13 +4306,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4356,25 +4350,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2" t="s">
         <v>132</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
         <v>134</v>
-      </c>
-      <c r="F2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" t="s">
-        <v>137</v>
       </c>
       <c r="I2">
         <v>18</v>
@@ -4418,25 +4412,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -4507,13 +4501,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4555,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBB5582-C584-406A-ABB8-AA0332D414F1}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4582,13 +4576,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4632,7 +4626,7 @@
         <v>2015</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4641,10 +4635,10 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I2">
         <v>23</v>
@@ -4689,25 +4683,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -4751,25 +4745,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C4">
         <v>2014</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -4813,25 +4807,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="D5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -4873,25 +4867,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C6">
         <v>2007</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="H6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -4935,25 +4929,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F7" t="s">
         <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -4997,19 +4991,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C8">
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I8">
         <v>8</v>
@@ -5053,25 +5047,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G9" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H9" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I9">
         <v>25</v>
@@ -5113,25 +5107,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C10">
         <v>2020</v>
       </c>
       <c r="D10" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E10" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G10" t="s">
         <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I10">
         <f>30*2</f>
@@ -5175,25 +5169,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C11">
         <v>2013</v>
       </c>
       <c r="D11" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="H11" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I11">
         <f>10*10</f>
@@ -5237,25 +5231,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C12">
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E12" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="G12" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="H12" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -5297,25 +5291,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C13">
         <v>2020</v>
       </c>
       <c r="D13" t="s">
+        <v>403</v>
+      </c>
+      <c r="E13" t="s">
+        <v>381</v>
+      </c>
+      <c r="F13" t="s">
         <v>408</v>
       </c>
-      <c r="E13" t="s">
-        <v>386</v>
-      </c>
-      <c r="F13" t="s">
-        <v>146</v>
-      </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H13" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -5384,13 +5378,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5446,7 +5440,7 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -5515,13 +5509,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -5559,22 +5553,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I2">
         <v>15</v>
@@ -5616,19 +5610,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="I3">
         <v>6</v>
@@ -5670,25 +5664,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C4">
         <v>2011</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -5730,19 +5724,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C5">
         <v>2010</v>
       </c>
       <c r="D5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I5">
         <v>10</v>
@@ -5786,19 +5780,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C6">
         <v>2009</v>
       </c>
       <c r="D6" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E6" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="H6" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I6">
         <v>8</v>
@@ -5841,19 +5835,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C7">
         <v>2008</v>
       </c>
       <c r="D7" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E7" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="H7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I7">
         <v>8</v>
@@ -5897,22 +5891,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E8" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="G8" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="H8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="I8">
         <v>12</v>
@@ -5956,25 +5950,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G9" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H9" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I9">
         <v>22</v>
@@ -6018,25 +6012,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C10">
         <v>2014</v>
       </c>
       <c r="D10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" t="s">
         <v>253</v>
       </c>
-      <c r="F10" t="s">
-        <v>258</v>
-      </c>
       <c r="G10" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H10" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I10">
         <v>29</v>
@@ -6083,12 +6077,13 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -6108,13 +6103,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -6152,25 +6147,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C2">
         <v>2007</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I2">
         <v>14</v>
@@ -6226,7 +6221,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>39</v>
@@ -6286,13 +6281,13 @@
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -6334,25 +6329,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
         <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -6394,22 +6389,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>409</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="H6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -6451,25 +6446,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C7">
         <v>2017</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I7">
         <v>24</v>
@@ -6519,16 +6514,16 @@
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -6571,25 +6566,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C9">
         <v>2013</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -6633,25 +6628,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C10">
         <v>2009</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F10" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H10" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -6695,22 +6690,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C11">
         <v>2015</v>
       </c>
       <c r="D11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F11" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G11" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -6752,25 +6747,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" t="s">
         <v>226</v>
-      </c>
-      <c r="E12" t="s">
-        <v>227</v>
-      </c>
-      <c r="F12" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" t="s">
-        <v>229</v>
-      </c>
-      <c r="H12" t="s">
-        <v>231</v>
       </c>
       <c r="I12">
         <v>42</v>
@@ -6820,19 +6815,19 @@
         <v>2016</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="G13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I13">
         <f>(14/18)*135</f>
@@ -6875,25 +6870,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C14">
         <v>2011</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I14">
         <v>9</v>
@@ -6941,7 +6936,7 @@
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -6950,10 +6945,10 @@
         <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H15" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I15">
         <v>23</v>
@@ -6997,25 +6992,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -7059,25 +7054,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C17">
         <v>2010</v>
       </c>
       <c r="D17" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E17" t="s">
         <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H17" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I17">
         <v>11</v>
@@ -7121,25 +7116,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C18">
         <v>2014</v>
       </c>
       <c r="D18" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H18" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I18">
         <v>11</v>
@@ -7181,16 +7176,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C19">
         <v>2022</v>
       </c>
       <c r="D19" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E19" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F19" t="s">
         <v>72</v>
@@ -7199,7 +7194,7 @@
         <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I19">
         <v>10</v>
@@ -7243,25 +7238,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C20">
         <v>2014</v>
       </c>
       <c r="D20" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E20" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F20" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G20" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="H20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I20">
         <v>6</v>
@@ -7303,25 +7298,25 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C21">
         <v>2020</v>
       </c>
       <c r="D21" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G21" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H21" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I21">
         <v>6</v>
@@ -7364,25 +7359,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C22">
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E22" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F22" t="s">
         <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I22">
         <v>9</v>
@@ -7424,25 +7419,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C23">
         <v>2022</v>
       </c>
       <c r="D23" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E23" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="F23" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G23" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H23" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="I23">
         <f>13*9</f>
@@ -7486,25 +7481,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C24">
         <v>2006</v>
       </c>
       <c r="D24" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E24" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F24" t="s">
         <v>72</v>
       </c>
       <c r="G24" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="H24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -7548,25 +7543,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C25">
         <v>2019</v>
       </c>
       <c r="D25" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E25" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F25" t="s">
         <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H25" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I25">
         <v>20</v>
@@ -7613,7 +7608,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7638,13 +7633,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7682,13 +7677,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -7697,10 +7692,10 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -7742,25 +7737,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I3">
         <v>14</v>
@@ -7802,22 +7797,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C4">
         <v>2006</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -7859,25 +7854,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I5">
         <v>15</v>
@@ -7921,25 +7916,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I6">
         <v>24</v>
@@ -7995,13 +7990,13 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="G7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I7">
         <f>5*3</f>
@@ -8051,16 +8046,16 @@
         <v>2013</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I8">
         <v>11</v>
@@ -8104,19 +8099,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E9" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H9" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I9">
         <v>21</v>
@@ -8158,25 +8153,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G10" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H10" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -8220,25 +8215,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
         <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -8280,25 +8275,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" t="s">
         <v>226</v>
-      </c>
-      <c r="E12" t="s">
-        <v>227</v>
-      </c>
-      <c r="F12" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" t="s">
-        <v>229</v>
-      </c>
-      <c r="H12" t="s">
-        <v>231</v>
       </c>
       <c r="I12">
         <v>42</v>
@@ -8342,25 +8337,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C13">
         <v>2016</v>
       </c>
       <c r="D13" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E13" t="s">
         <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H13" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="I13">
         <v>6</v>
@@ -8404,25 +8399,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C14">
         <v>2014</v>
       </c>
       <c r="D14" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E14" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G14" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="H14" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -8464,25 +8459,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C15">
         <v>2020</v>
       </c>
       <c r="D15" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G15" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H15" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -8525,25 +8520,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E16" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F16" t="s">
         <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H16" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I16">
         <v>9</v>
@@ -8585,25 +8580,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C17">
         <v>2022</v>
       </c>
       <c r="D17" t="s">
+        <v>385</v>
+      </c>
+      <c r="E17" t="s">
+        <v>386</v>
+      </c>
+      <c r="F17" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" t="s">
+        <v>387</v>
+      </c>
+      <c r="H17" t="s">
         <v>390</v>
-      </c>
-      <c r="E17" t="s">
-        <v>391</v>
-      </c>
-      <c r="F17" t="s">
-        <v>258</v>
-      </c>
-      <c r="G17" t="s">
-        <v>392</v>
-      </c>
-      <c r="H17" t="s">
-        <v>395</v>
       </c>
       <c r="I17">
         <f>13*9</f>
@@ -8677,13 +8672,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -8736,10 +8731,10 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -8783,25 +8778,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C3">
         <v>2015</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E3" t="s">
         <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -8843,25 +8838,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C4">
         <v>2015</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -8905,25 +8900,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -8967,25 +8962,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C6">
         <v>2013</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I6">
         <v>16</v>
@@ -9029,25 +9024,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I7">
         <v>42</v>
@@ -9091,25 +9086,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="I8">
         <v>10</v>
@@ -9151,25 +9146,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C9">
         <v>2020</v>
       </c>
       <c r="D9" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9" t="s">
+        <v>381</v>
+      </c>
+      <c r="F9" t="s">
         <v>408</v>
       </c>
-      <c r="E9" t="s">
-        <v>386</v>
-      </c>
-      <c r="F9" t="s">
-        <v>146</v>
-      </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H9" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I9">
         <v>11</v>
@@ -9241,13 +9236,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -9285,25 +9280,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C2">
         <v>2001</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G2" t="s">
         <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -9345,25 +9340,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
         <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -9465,25 +9460,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5">
         <v>2003</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I5">
         <v>16</v>
@@ -9539,13 +9534,13 @@
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I6">
         <v>15</v>
@@ -9587,25 +9582,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7">
         <v>2007</v>
       </c>
       <c r="D7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I7">
         <v>14</v>
@@ -9649,25 +9644,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C8">
         <v>2007</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -9709,19 +9704,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C9">
         <v>2021</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>409</v>
       </c>
       <c r="E9" t="s">
         <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I9">
         <f>2*12</f>
@@ -9771,19 +9766,19 @@
         <v>2016</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="G10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I10">
         <f>(14/18)*135</f>
@@ -9826,25 +9821,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I11">
         <v>6</v>
@@ -9892,16 +9887,16 @@
         <v>2013</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I12">
         <v>11</v>
@@ -9944,25 +9939,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C13">
         <v>2014</v>
       </c>
       <c r="D13" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H13" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -10004,16 +9999,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C14">
         <v>2022</v>
       </c>
       <c r="D14" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E14" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F14" t="s">
         <v>72</v>
@@ -10022,7 +10017,7 @@
         <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I14">
         <v>10</v>
@@ -10066,25 +10061,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C15">
         <v>2021</v>
       </c>
       <c r="D15" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E15" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F15" t="s">
         <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H15" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I15">
         <v>9</v>
@@ -10126,25 +10121,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C16">
         <v>2006</v>
       </c>
       <c r="D16" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E16" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F16" t="s">
         <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="H16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I16">
         <v>10</v>
@@ -10188,25 +10183,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C17">
         <v>2019</v>
       </c>
       <c r="D17" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E17" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F17" t="s">
         <v>72</v>
       </c>
       <c r="G17" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H17" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I17">
         <v>20</v>
@@ -10253,7 +10248,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10278,13 +10273,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -10322,13 +10317,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C2">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -10337,10 +10332,10 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I2">
         <v>36</v>
@@ -10382,22 +10377,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C3">
         <v>2006</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -10439,25 +10434,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -10501,25 +10496,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I5">
         <v>22</v>
@@ -10563,13 +10558,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -10578,10 +10573,10 @@
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -10623,25 +10618,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C7">
         <v>2013</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I7">
         <v>16</v>
@@ -10683,22 +10678,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I8">
         <v>13</v>
@@ -10740,25 +10735,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="G9" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -10814,13 +10809,13 @@
         <v>97</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
         <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I10">
         <v>32</v>
@@ -10876,13 +10871,13 @@
         <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H11" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I11">
         <v>28</v>
@@ -10926,19 +10921,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>301</v>
       </c>
       <c r="I12">
         <v>717</v>
@@ -10980,25 +10975,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -11042,25 +11037,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C14">
         <v>2016</v>
       </c>
       <c r="D14" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E14" t="s">
         <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G14" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H14" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -11103,25 +11098,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C15">
         <v>2022</v>
       </c>
       <c r="D15" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E15" t="s">
+        <v>386</v>
+      </c>
+      <c r="F15" t="s">
+        <v>253</v>
+      </c>
+      <c r="G15" t="s">
+        <v>387</v>
+      </c>
+      <c r="H15" t="s">
         <v>391</v>
-      </c>
-      <c r="F15" t="s">
-        <v>258</v>
-      </c>
-      <c r="G15" t="s">
-        <v>392</v>
-      </c>
-      <c r="H15" t="s">
-        <v>396</v>
       </c>
       <c r="I15">
         <f>13*9</f>
@@ -11195,13 +11190,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -11239,25 +11234,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -11301,19 +11296,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C3">
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I3">
         <v>21</v>
@@ -11355,25 +11350,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C4">
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -11417,25 +11412,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C5">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I5">
         <v>14</v>
@@ -11477,13 +11472,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C6">
         <v>2021</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -11492,10 +11487,10 @@
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -11539,25 +11534,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
       <c r="D7" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E7" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F7" t="s">
-        <v>146</v>
+        <v>408</v>
       </c>
       <c r="G7" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="H7" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -11599,25 +11594,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C8">
         <v>2020</v>
       </c>
       <c r="D8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H8" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -11660,25 +11655,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C9">
         <v>2021</v>
       </c>
       <c r="D9" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E9" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F9" t="s">
         <v>72</v>
       </c>
       <c r="G9" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H9" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I9">
         <v>9</v>
@@ -11747,13 +11742,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -11863,7 +11858,7 @@
         <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>83</v>
@@ -11941,13 +11936,13 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -12058,7 +12053,7 @@
         <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>91</v>
@@ -12172,7 +12167,7 @@
         <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G5" t="s">
         <v>99</v>
@@ -12279,25 +12274,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C7">
         <v>2022</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -12341,25 +12336,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C8">
         <v>2021</v>
       </c>
       <c r="D8" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E8" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F8" t="s">
         <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H8" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I8">
         <v>9</v>

</xml_diff>